<commit_message>
impliment the reprocessing of old data points
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_ctr.xlsx
+++ b/dump_files/temp_data_ctr.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AD23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,25 +518,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>9250</v>
+        <v>9611</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.5873437500000001</v>
+        <v>-0.67375</v>
       </c>
       <c r="E2" t="n">
-        <v>0.003046875</v>
+        <v>0.0025</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06072529069660132</v>
+        <v>0.05540122431794699</v>
       </c>
       <c r="G2" t="n">
-        <v>0.003386093586507148</v>
+        <v>0.002132268347967683</v>
       </c>
       <c r="H2" t="n">
-        <v>3.821848206843504e-05</v>
+        <v>2.960257384351209e-05</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3000003264736568</v>
+        <v>0.3000012738921269</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -554,19 +554,19 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>16.10676874999999</v>
+        <v>22.47166875</v>
       </c>
       <c r="O2" t="n">
-        <v>2.5609</v>
+        <v>2.555074999999999</v>
       </c>
       <c r="P2" t="n">
-        <v>12.39335</v>
+        <v>12.3946</v>
       </c>
       <c r="Q2" t="n">
         <v>2</v>
       </c>
       <c r="R2" t="n">
-        <v>221104</v>
+        <v>434767</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="AD2" t="n">
-        <v>0.01254218537885074</v>
+        <v>0.008402738950133338</v>
       </c>
     </row>
     <row r="3">
@@ -614,25 +614,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>9250</v>
+        <v>9611</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.588828125</v>
+        <v>-0.676640625</v>
       </c>
       <c r="E3" t="n">
-        <v>0.003359375</v>
+        <v>0.00453125</v>
       </c>
       <c r="F3" t="n">
-        <v>0.06502492974434324</v>
+        <v>0.06072664546190596</v>
       </c>
       <c r="G3" t="n">
-        <v>0.003403152611354065</v>
+        <v>0.002140657011737251</v>
       </c>
       <c r="H3" t="n">
-        <v>3.808487633236006e-05</v>
+        <v>2.965385334721703e-05</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3400007063970575</v>
+        <v>0.3399996740020741</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -650,19 +650,19 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>16.12913124999999</v>
+        <v>22.49151875</v>
       </c>
       <c r="O3" t="n">
-        <v>2.910249999999998</v>
+        <v>2.904399999999999</v>
       </c>
       <c r="P3" t="n">
-        <v>12.3968875</v>
+        <v>12.398275</v>
       </c>
       <c r="Q3" t="n">
         <v>2</v>
       </c>
       <c r="R3" t="n">
-        <v>219570</v>
+        <v>432695</v>
       </c>
       <c r="S3" t="n">
         <v>1</v>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="AD3" t="n">
-        <v>0.01194192300841409</v>
+        <v>0.007854079331334972</v>
       </c>
     </row>
     <row r="4">
@@ -710,25 +710,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>9250</v>
+        <v>9611</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.57234375</v>
+        <v>-0.67984375</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002890625</v>
+        <v>0.003984375</v>
       </c>
       <c r="F4" t="n">
-        <v>0.07118473868171747</v>
+        <v>0.07423428617036767</v>
       </c>
       <c r="G4" t="n">
-        <v>0.003404056432806439</v>
+        <v>0.002134818713205991</v>
       </c>
       <c r="H4" t="n">
-        <v>3.807349990868614e-05</v>
+        <v>2.942804687693398e-05</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -737,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3799996762620905</v>
+        <v>0.3799990896676447</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -746,19 +746,19 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>16.16121875</v>
+        <v>22.52130624999999</v>
       </c>
       <c r="O4" t="n">
-        <v>3.259625</v>
+        <v>3.253775000000001</v>
       </c>
       <c r="P4" t="n">
-        <v>12.400625</v>
+        <v>12.402175</v>
       </c>
       <c r="Q4" t="n">
         <v>2</v>
       </c>
       <c r="R4" t="n">
-        <v>219836</v>
+        <v>436876</v>
       </c>
       <c r="S4" t="n">
         <v>1</v>
@@ -798,7 +798,7 @@
         </is>
       </c>
       <c r="AD4" t="n">
-        <v>0.01147729850021075</v>
+        <v>0.009029122541334986</v>
       </c>
     </row>
     <row r="5">
@@ -806,25 +806,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>9250</v>
+        <v>9611</v>
       </c>
       <c r="C5" t="n">
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.58625</v>
+        <v>-0.69828125</v>
       </c>
       <c r="E5" t="n">
-        <v>0.003125</v>
+        <v>0.0025</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0751473843883417</v>
+        <v>0.08819426140829709</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00338620184077266</v>
+        <v>0.002142785320123611</v>
       </c>
       <c r="H5" t="n">
-        <v>3.771685805651443e-05</v>
+        <v>2.942974989624887e-05</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4200003958923806</v>
+        <v>0.4199990537942545</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -842,19 +842,19 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>16.20329374999999</v>
+        <v>22.56095625</v>
       </c>
       <c r="O5" t="n">
-        <v>3.60905</v>
+        <v>3.603200000000001</v>
       </c>
       <c r="P5" t="n">
-        <v>12.404625</v>
+        <v>12.4063</v>
       </c>
       <c r="Q5" t="n">
         <v>2</v>
       </c>
       <c r="R5" t="n">
-        <v>221518</v>
+        <v>437300</v>
       </c>
       <c r="S5" t="n">
         <v>1</v>
@@ -894,7 +894,1735 @@
         </is>
       </c>
       <c r="AD5" t="n">
-        <v>0.01285062737431644</v>
+        <v>0.008313644437592214</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.671796875</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.003515625</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1120522703396545</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.002166057148703684</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.940483083196337e-05</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.4600001765346823</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>22.61067499999999</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3.9526875</v>
+      </c>
+      <c r="P6" t="n">
+        <v>12.4107</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2</v>
+      </c>
+      <c r="R6" t="n">
+        <v>434858</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" t="n">
+        <v>60</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>180</v>
+      </c>
+      <c r="X6" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.007901959627160842</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.68578125</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.00296875</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1351768603019902</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.002173575902483256</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.917164362174072e-05</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5000012233485214</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>22.67028125</v>
+      </c>
+      <c r="O7" t="n">
+        <v>4.3022375</v>
+      </c>
+      <c r="P7" t="n">
+        <v>12.4153</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2</v>
+      </c>
+      <c r="R7" t="n">
+        <v>436177</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" t="n">
+        <v>60</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>180</v>
+      </c>
+      <c r="X7" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.007749108027912011</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.674296875</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.00375</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1679439286399889</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.002211121303288534</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.924366874210862e-05</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.5400049896433275</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>22.73975625</v>
+      </c>
+      <c r="O8" t="n">
+        <v>4.651875</v>
+      </c>
+      <c r="P8" t="n">
+        <v>12.4201125</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2</v>
+      </c>
+      <c r="R8" t="n">
+        <v>431055</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" t="b">
+        <v>1</v>
+      </c>
+      <c r="U8" t="n">
+        <v>60</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>180</v>
+      </c>
+      <c r="X8" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.008640887233368739</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.674921875</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.005546875</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.1993190003861794</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.002220975442324475</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3.021366864648573e-05</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.579998095832036</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>22.81931874999999</v>
+      </c>
+      <c r="O9" t="n">
+        <v>5.0016</v>
+      </c>
+      <c r="P9" t="n">
+        <v>12.4252375</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>2</v>
+      </c>
+      <c r="R9" t="n">
+        <v>430971</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
+        <v>60</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>180</v>
+      </c>
+      <c r="X9" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.008375162811860227</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.676015625</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0034375</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.2376202034104397</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.002257317934687978</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3.021366864648573e-05</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.6200002082984606</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>22.90873125</v>
+      </c>
+      <c r="O10" t="n">
+        <v>5.351475000000001</v>
+      </c>
+      <c r="P10" t="n">
+        <v>12.430475</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2</v>
+      </c>
+      <c r="R10" t="n">
+        <v>431395</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" t="b">
+        <v>1</v>
+      </c>
+      <c r="U10" t="n">
+        <v>60</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>180</v>
+      </c>
+      <c r="X10" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.009425091446127704</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.679609375</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.001328125</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.2842753032444323</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.002292676194735253</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.021366864648573e-05</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.6599988197013554</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>23.008075</v>
+      </c>
+      <c r="O11" t="n">
+        <v>5.701437500000001</v>
+      </c>
+      <c r="P11" t="n">
+        <v>12.4358875</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" t="n">
+        <v>438162</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" t="b">
+        <v>1</v>
+      </c>
+      <c r="U11" t="n">
+        <v>60</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>180</v>
+      </c>
+      <c r="X11" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.01022565417319077</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.68703125</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3375422867814002</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.002338084171359591</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3.093581626698153e-05</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.69999958504686</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>23.117375</v>
+      </c>
+      <c r="O12" t="n">
+        <v>6.051562499999999</v>
+      </c>
+      <c r="P12" t="n">
+        <v>12.4414875</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2</v>
+      </c>
+      <c r="R12" t="n">
+        <v>436640</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="n">
+        <v>60</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>180</v>
+      </c>
+      <c r="X12" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.01046721455475502</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.682578125</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.005703125</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.4162242730783579</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.002390423134099924</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3.198287119811531e-05</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.7400015392169229</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>23.23663749999999</v>
+      </c>
+      <c r="O13" t="n">
+        <v>6.401837499999999</v>
+      </c>
+      <c r="P13" t="n">
+        <v>12.447275</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2</v>
+      </c>
+      <c r="R13" t="n">
+        <v>435531</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" t="n">
+        <v>60</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>180</v>
+      </c>
+      <c r="X13" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.009838119079429761</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.68671875</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.001328125</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.3993505204491841</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.001369928608764267</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3.143849235934305e-05</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.7799986233308355</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>23.36583125</v>
+      </c>
+      <c r="O14" t="n">
+        <v>6.752262500000001</v>
+      </c>
+      <c r="P14" t="n">
+        <v>12.4532</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2</v>
+      </c>
+      <c r="R14" t="n">
+        <v>435923</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" t="b">
+        <v>1</v>
+      </c>
+      <c r="U14" t="n">
+        <v>60</v>
+      </c>
+      <c r="V14" t="n">
+        <v>105</v>
+      </c>
+      <c r="W14" t="n">
+        <v>180</v>
+      </c>
+      <c r="X14" t="n">
+        <v>70</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.003358366838110744</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.6782812500000001</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.00125</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5823476342890446</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.001527177103557801</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3.201858034904118e-05</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.8200007602135166</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>23.50501875</v>
+      </c>
+      <c r="O15" t="n">
+        <v>7.102887499999998</v>
+      </c>
+      <c r="P15" t="n">
+        <v>12.4592875</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>2</v>
+      </c>
+      <c r="R15" t="n">
+        <v>434581</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" t="b">
+        <v>1</v>
+      </c>
+      <c r="U15" t="n">
+        <v>60</v>
+      </c>
+      <c r="V15" t="n">
+        <v>105</v>
+      </c>
+      <c r="W15" t="n">
+        <v>180</v>
+      </c>
+      <c r="X15" t="n">
+        <v>70</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD15" t="n">
+        <v>0.003645701800541045</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.684296875</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.005234375</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.075563777534186</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.002781736753866347</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3.365543120374141e-05</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.8600011656062164</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>23.654225</v>
+      </c>
+      <c r="O16" t="n">
+        <v>7.453687500000001</v>
+      </c>
+      <c r="P16" t="n">
+        <v>12.4655125</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>2</v>
+      </c>
+      <c r="R16" t="n">
+        <v>434639</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1</v>
+      </c>
+      <c r="T16" t="b">
+        <v>1</v>
+      </c>
+      <c r="U16" t="n">
+        <v>60</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>180</v>
+      </c>
+      <c r="X16" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.01186750296541475</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>9611</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.672109375</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.002265625</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.873514074889714</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.003270423969317405</v>
+      </c>
+      <c r="H17" t="n">
+        <v>3.758797925048509e-05</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.8999995844849702</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>23.81348125</v>
+      </c>
+      <c r="O17" t="n">
+        <v>7.8046875</v>
+      </c>
+      <c r="P17" t="n">
+        <v>12.4718375</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>2</v>
+      </c>
+      <c r="R17" t="n">
+        <v>434609</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" t="b">
+        <v>1</v>
+      </c>
+      <c r="U17" t="n">
+        <v>60</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" t="n">
+        <v>180</v>
+      </c>
+      <c r="X17" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD17" t="n">
+        <v>0.01307180990242717</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>9612</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.68015625</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0034375</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.541860005171722</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.002218753826434185</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4.046564216982621e-05</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1.099999752850983</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>24.76000625</v>
+      </c>
+      <c r="O18" t="n">
+        <v>9.563324999999999</v>
+      </c>
+      <c r="P18" t="n">
+        <v>12.5045625</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>2</v>
+      </c>
+      <c r="R18" t="n">
+        <v>437042</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" t="b">
+        <v>1</v>
+      </c>
+      <c r="U18" t="n">
+        <v>64</v>
+      </c>
+      <c r="V18" t="n">
+        <v>145</v>
+      </c>
+      <c r="W18" t="n">
+        <v>180</v>
+      </c>
+      <c r="X18" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD18" t="n">
+        <v>0.00426808319115972</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>9612</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.67390625</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9835268230263811</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.001865392499449286</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3.435188701997838e-05</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.11999730804813</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>24.86854374999999</v>
+      </c>
+      <c r="O19" t="n">
+        <v>9.739549999999999</v>
+      </c>
+      <c r="P19" t="n">
+        <v>12.5078625</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>2</v>
+      </c>
+      <c r="R19" t="n">
+        <v>437054</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1</v>
+      </c>
+      <c r="T19" t="b">
+        <v>1</v>
+      </c>
+      <c r="U19" t="n">
+        <v>64</v>
+      </c>
+      <c r="V19" t="n">
+        <v>145</v>
+      </c>
+      <c r="W19" t="n">
+        <v>180</v>
+      </c>
+      <c r="X19" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD19" t="n">
+        <v>0.00431358635796269</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>9612</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.680078125</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.6860523061909166</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.001645656706061005</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3.148140936903561e-05</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.139999540941444</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>24.979525</v>
+      </c>
+      <c r="O20" t="n">
+        <v>9.9158875</v>
+      </c>
+      <c r="P20" t="n">
+        <v>12.511175</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>2</v>
+      </c>
+      <c r="R20" t="n">
+        <v>436561</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1</v>
+      </c>
+      <c r="T20" t="b">
+        <v>1</v>
+      </c>
+      <c r="U20" t="n">
+        <v>64</v>
+      </c>
+      <c r="V20" t="n">
+        <v>154</v>
+      </c>
+      <c r="W20" t="n">
+        <v>180</v>
+      </c>
+      <c r="X20" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.004232168411078725</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>9612</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.68953125</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.005468750000000001</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.4954066039462818</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.001484798113005253</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2.886711365702827e-05</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1.160000919607416</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>25.09306249999999</v>
+      </c>
+      <c r="O21" t="n">
+        <v>10.09225</v>
+      </c>
+      <c r="P21" t="n">
+        <v>12.5144375</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>2</v>
+      </c>
+      <c r="R21" t="n">
+        <v>435323</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" t="b">
+        <v>1</v>
+      </c>
+      <c r="U21" t="n">
+        <v>64</v>
+      </c>
+      <c r="V21" t="n">
+        <v>154</v>
+      </c>
+      <c r="W21" t="n">
+        <v>180</v>
+      </c>
+      <c r="X21" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.00391750504067894</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>9612</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0.684765625</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.000390625</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.3955017484483202</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.002208881391804533</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2.545900886436236e-05</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1.180001053982441</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>25.20906249999999</v>
+      </c>
+      <c r="O22" t="n">
+        <v>10.268725</v>
+      </c>
+      <c r="P22" t="n">
+        <v>12.5177375</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>2</v>
+      </c>
+      <c r="R22" t="n">
+        <v>434309</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1</v>
+      </c>
+      <c r="T22" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" t="n">
+        <v>60</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>180</v>
+      </c>
+      <c r="X22" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD22" t="n">
+        <v>0.009170489260956325</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>9612</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-0.6840625</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0028125</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.3037246884330189</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.002123139562965389</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2.545900886436236e-05</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1.199998158009192</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>25.32764375</v>
+      </c>
+      <c r="O23" t="n">
+        <v>10.44525</v>
+      </c>
+      <c r="P23" t="n">
+        <v>12.5210125</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>2</v>
+      </c>
+      <c r="R23" t="n">
+        <v>433212</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1</v>
+      </c>
+      <c r="T23" t="b">
+        <v>1</v>
+      </c>
+      <c r="U23" t="n">
+        <v>60</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>180</v>
+      </c>
+      <c r="X23" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD23" t="n">
+        <v>0.008464852229313695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make more user-friendly the config file reader in ubmate: unfinished yet
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_ctr.xlsx
+++ b/dump_files/temp_data_ctr.xlsx
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,125 +446,135 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>potential</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>current</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>peak_intensity</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>peak_intensity_error</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>bkg</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>phi</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>chi</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>mu</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>del</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>nu</t>
-        </is>
-      </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>eta</t>
+          <t>delta</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>norm</t>
+          <t>gamma</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>transmission</t>
+          <t>omega_t</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>mon</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>transm</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>mask_ctr</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>roi_x</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>roi_y</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>roi_w</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>roi_h</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>ss_factor</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>peak_width</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>poly_func</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>poly_order</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>poly_type</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>noise</t>
         </is>
@@ -576,359 +585,95 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>239</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0411445936210609</v>
+        <v>0.370234375</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002184679322998997</v>
+        <v>-0.031171875</v>
       </c>
       <c r="F2" t="n">
-        <v>9.786115364982134e-05</v>
+        <v>-0.01931891553061071</v>
       </c>
       <c r="G2" t="n">
+        <v>0.0348895910479822</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.001047952575534606</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.09999962720421532</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>15.23426875</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.3986249999999991</v>
+      </c>
+      <c r="P2" t="n">
+        <v>12.7822875</v>
+      </c>
+      <c r="Q2" t="n">
         <v>2</v>
       </c>
-      <c r="H2" t="n">
+      <c r="R2" t="n">
+        <v>81738</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>80</v>
+      </c>
+      <c r="V2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-146.6508</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.0669</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.9095</v>
-      </c>
-      <c r="M2" t="n">
-        <v>21.6689</v>
-      </c>
-      <c r="N2" t="n">
-        <v>11.886</v>
-      </c>
-      <c r="O2" t="n">
-        <v>10.8345</v>
-      </c>
-      <c r="P2" t="n">
-        <v>130600</v>
-      </c>
-      <c r="Q2" t="n">
+      <c r="W2" t="n">
+        <v>240</v>
+      </c>
+      <c r="X2" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB2" t="n">
         <v>1</v>
       </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>20</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>60</v>
-      </c>
-      <c r="V2" t="n">
-        <v>100</v>
-      </c>
-      <c r="W2" t="n">
-        <v>2</v>
-      </c>
-      <c r="X2" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>atq</t>
-        </is>
-      </c>
-      <c r="Z2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>traditional</t>
         </is>
       </c>
-      <c r="AB2" t="n">
-        <v>0.009011114999147515</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>12</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.04404060971237923</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.002227629629309023</v>
-      </c>
-      <c r="F3" t="n">
-        <v>9.746839463820597e-05</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="J3" t="n">
-        <v>-146.2289</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.0746</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.9085</v>
-      </c>
-      <c r="M3" t="n">
-        <v>21.6295</v>
-      </c>
-      <c r="N3" t="n">
-        <v>12.84875</v>
-      </c>
-      <c r="O3" t="n">
-        <v>10.8157</v>
-      </c>
-      <c r="P3" t="n">
-        <v>125928</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S3" t="n">
-        <v>20</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>60</v>
-      </c>
-      <c r="V3" t="n">
-        <v>100</v>
-      </c>
-      <c r="W3" t="n">
-        <v>2</v>
-      </c>
-      <c r="X3" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>atq</t>
-        </is>
-      </c>
-      <c r="Z3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>traditional</t>
-        </is>
-      </c>
-      <c r="AB3" t="n">
-        <v>0.007954771784600599</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>12</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.05525468122538955</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.002228304770188015</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9.699502925354997e-05</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.74</v>
-      </c>
-      <c r="J4" t="n">
-        <v>-145.7663</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.08309999999999999</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.9075</v>
-      </c>
-      <c r="M4" t="n">
-        <v>21.5853</v>
-      </c>
-      <c r="N4" t="n">
-        <v>13.82375</v>
-      </c>
-      <c r="O4" t="n">
-        <v>10.7946</v>
-      </c>
-      <c r="P4" t="n">
-        <v>127278</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4" t="n">
-        <v>20</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>60</v>
-      </c>
-      <c r="V4" t="n">
-        <v>100</v>
-      </c>
-      <c r="W4" t="n">
-        <v>2</v>
-      </c>
-      <c r="X4" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>atq</t>
-        </is>
-      </c>
-      <c r="Z4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>traditional</t>
-        </is>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.008620549848475028</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.06329474888846222</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.002637828808149997</v>
-      </c>
-      <c r="F5" t="n">
-        <v>9.537067485110892e-05</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-145.603</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.08599999999999999</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.9075</v>
-      </c>
-      <c r="M5" t="n">
-        <v>21.5718</v>
-      </c>
-      <c r="N5" t="n">
-        <v>14.154</v>
-      </c>
-      <c r="O5" t="n">
-        <v>10.787</v>
-      </c>
-      <c r="P5" t="n">
-        <v>91230</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S5" t="n">
-        <v>20</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>60</v>
-      </c>
-      <c r="V5" t="n">
-        <v>100</v>
-      </c>
-      <c r="W5" t="n">
-        <v>2</v>
-      </c>
-      <c r="X5" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>atq</t>
-        </is>
-      </c>
-      <c r="Z5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>traditional</t>
-        </is>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.01098118131001881</v>
+      <c r="AD2" t="n">
+        <v>0.2528706243591782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish debugging + add possibility to change primary beam position
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_ctr.xlsx
+++ b/dump_files/temp_data_ctr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AD21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,6 +676,1830 @@
         <v>0.2528706243591782</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>239</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.369921875</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.030234375</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0306686203528263</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.03602083406320463</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.001115638389705981</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.1168567663976847</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>15.2269125</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.4739874999999998</v>
+      </c>
+      <c r="P3" t="n">
+        <v>12.782675</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" t="n">
+        <v>81697</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" t="n">
+        <v>80</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>240</v>
+      </c>
+      <c r="X3" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.2555131608366457</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>239</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.366640625</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.030546875</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.02538906832280519</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.03720528146606428</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.001193052423908981</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.133714192847559</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>15.2199875</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.5493500000000004</v>
+      </c>
+      <c r="P4" t="n">
+        <v>12.7830125</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R4" t="n">
+        <v>81921</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" t="n">
+        <v>80</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>240</v>
+      </c>
+      <c r="X4" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.2633941905062686</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>239</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.369765625</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.029609375</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.01924925155299173</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.03818773999634662</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.00125212764901426</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.1505722772438844</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>15.2135125</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.6247125000000011</v>
+      </c>
+      <c r="P5" t="n">
+        <v>12.783375</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2</v>
+      </c>
+      <c r="R5" t="n">
+        <v>81551</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="b">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
+        <v>80</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>240</v>
+      </c>
+      <c r="X5" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.2877566101127563</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>239</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.369921875</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.030546875</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0132016711176316</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.03931455150237265</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.001327559656561201</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.1674281367478578</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>15.20748125</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.7000625000000014</v>
+      </c>
+      <c r="P6" t="n">
+        <v>12.7837375</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2</v>
+      </c>
+      <c r="R6" t="n">
+        <v>81606</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" t="n">
+        <v>80</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>240</v>
+      </c>
+      <c r="X6" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.2898000309178211</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>239</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.364375</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.030078125</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.03210029539423864</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.04025118189478549</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.001391693855284749</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1842844621302785</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>15.2019</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.7754124999999981</v>
+      </c>
+      <c r="P7" t="n">
+        <v>12.7841125</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2</v>
+      </c>
+      <c r="R7" t="n">
+        <v>81573</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" t="n">
+        <v>80</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>240</v>
+      </c>
+      <c r="X7" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.3131419648654402</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>239</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.366640625</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.030703125</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.03400019037309654</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.04096716402005959</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.001435494105203144</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.2011440730560368</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>15.1968</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.8507749999999987</v>
+      </c>
+      <c r="P8" t="n">
+        <v>12.7845625</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2</v>
+      </c>
+      <c r="R8" t="n">
+        <v>81351</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" t="b">
+        <v>1</v>
+      </c>
+      <c r="U8" t="n">
+        <v>80</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>240</v>
+      </c>
+      <c r="X8" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.3106572341674902</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>239</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.366640625</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.032109375</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.02896574789263651</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.04161336255252465</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.00147992186103222</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.2179988775837056</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>15.19211875</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9261124999999986</v>
+      </c>
+      <c r="P9" t="n">
+        <v>12.784975</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>2</v>
+      </c>
+      <c r="R9" t="n">
+        <v>81235</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
+        <v>80</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>240</v>
+      </c>
+      <c r="X9" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.3155654168117988</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>239</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.361015625</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.029375</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.2058321333474415</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.04227625984806054</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.00152751423818033</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.2348562756886619</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>15.1879</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1.001462499999999</v>
+      </c>
+      <c r="P10" t="n">
+        <v>12.785425</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2</v>
+      </c>
+      <c r="R10" t="n">
+        <v>81145</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" t="b">
+        <v>1</v>
+      </c>
+      <c r="U10" t="n">
+        <v>80</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>240</v>
+      </c>
+      <c r="X10" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.3815628115860824</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>239</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.36890625</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.029609375</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6035854023273843</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0430058147279319</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.00158334154169437</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.2517145645450339</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>15.18411875</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.076812499999999</v>
+      </c>
+      <c r="P11" t="n">
+        <v>12.7858625</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" t="n">
+        <v>81218</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" t="b">
+        <v>1</v>
+      </c>
+      <c r="U11" t="n">
+        <v>80</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>240</v>
+      </c>
+      <c r="X11" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.5862182780120627</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>239</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.3675</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.668977048965846</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.04392894359311523</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.001646776263736264</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.2685729833361876</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>15.18080625</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.152162499999999</v>
+      </c>
+      <c r="P12" t="n">
+        <v>12.78635</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2</v>
+      </c>
+      <c r="R12" t="n">
+        <v>81250</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="n">
+        <v>80</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>240</v>
+      </c>
+      <c r="X12" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.990918566639563</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>239</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.370625</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.029296875</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4.098861696245788</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.04501944705799155</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.001708949597605758</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.2854287729450663</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>15.1779125</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1.227499999999999</v>
+      </c>
+      <c r="P13" t="n">
+        <v>12.7868</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2</v>
+      </c>
+      <c r="R13" t="n">
+        <v>81163</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" t="n">
+        <v>80</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>240</v>
+      </c>
+      <c r="X13" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD13" t="n">
+        <v>1.611268768680984</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>239</v>
+      </c>
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.361875</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.0309375</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8.88087698057652</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.04654371869581538</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.001782081825936057</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.3022854423339676</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>15.1754875</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1.302837499999999</v>
+      </c>
+      <c r="P14" t="n">
+        <v>12.7872875</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2</v>
+      </c>
+      <c r="R14" t="n">
+        <v>80950</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" t="b">
+        <v>1</v>
+      </c>
+      <c r="U14" t="n">
+        <v>80</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>240</v>
+      </c>
+      <c r="X14" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD14" t="n">
+        <v>2.509252152680931</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>239</v>
+      </c>
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.370859375</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.030234375</v>
+      </c>
+      <c r="F15" t="n">
+        <v>16.00730291485214</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.04825627587255936</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.001864375787849711</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.3191424903000004</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>15.1735</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1.378174999999999</v>
+      </c>
+      <c r="P15" t="n">
+        <v>12.7877875</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>2</v>
+      </c>
+      <c r="R15" t="n">
+        <v>80992</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" t="b">
+        <v>1</v>
+      </c>
+      <c r="U15" t="n">
+        <v>80</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>240</v>
+      </c>
+      <c r="X15" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD15" t="n">
+        <v>3.792077899815132</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>239</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.369609375</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.031328125</v>
+      </c>
+      <c r="F16" t="n">
+        <v>23.4083407150317</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0500391635749691</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.001959157574784081</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.3359993879820277</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>15.17195625</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1.453512499999999</v>
+      </c>
+      <c r="P16" t="n">
+        <v>12.788275</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>2</v>
+      </c>
+      <c r="R16" t="n">
+        <v>80933</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1</v>
+      </c>
+      <c r="T16" t="b">
+        <v>1</v>
+      </c>
+      <c r="U16" t="n">
+        <v>80</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>240</v>
+      </c>
+      <c r="X16" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD16" t="n">
+        <v>5.255371063644922</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>239</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.37078125</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.0290625</v>
+      </c>
+      <c r="F17" t="n">
+        <v>28.5494447612635</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.05132603881998209</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.002040197002927849</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.3528588305773088</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>15.170875</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1.528862499999999</v>
+      </c>
+      <c r="P17" t="n">
+        <v>12.7887875</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>2</v>
+      </c>
+      <c r="R17" t="n">
+        <v>80898</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" t="b">
+        <v>1</v>
+      </c>
+      <c r="U17" t="n">
+        <v>80</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" t="n">
+        <v>240</v>
+      </c>
+      <c r="X17" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD17" t="n">
+        <v>6.477585005165414</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>239</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.36671875</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.032109375</v>
+      </c>
+      <c r="F18" t="n">
+        <v>30.93209826031122</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.05205124327107966</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.002096872561102655</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.3697150955981949</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>15.17021875</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1.604199999999999</v>
+      </c>
+      <c r="P18" t="n">
+        <v>12.7892875</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>2</v>
+      </c>
+      <c r="R18" t="n">
+        <v>80906</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" t="b">
+        <v>1</v>
+      </c>
+      <c r="U18" t="n">
+        <v>80</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>240</v>
+      </c>
+      <c r="X18" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD18" t="n">
+        <v>7.231762505373693</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>239</v>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.3559375</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="F19" t="n">
+        <v>31.78572985225935</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.05246694150190739</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.002135958272314602</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.3865701411450752</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>15.1700125</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1.679524999999998</v>
+      </c>
+      <c r="P19" t="n">
+        <v>12.7898</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>2</v>
+      </c>
+      <c r="R19" t="n">
+        <v>80869</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1</v>
+      </c>
+      <c r="T19" t="b">
+        <v>1</v>
+      </c>
+      <c r="U19" t="n">
+        <v>80</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>240</v>
+      </c>
+      <c r="X19" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD19" t="n">
+        <v>7.710387309189457</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>239</v>
+      </c>
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.362265625</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.031328125</v>
+      </c>
+      <c r="F20" t="n">
+        <v>32.00348099783493</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.05283834540331669</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.002173428862770354</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.4034280257566321</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>15.17026875</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1.754862499999998</v>
+      </c>
+      <c r="P20" t="n">
+        <v>12.79035</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>2</v>
+      </c>
+      <c r="R20" t="n">
+        <v>80743</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1</v>
+      </c>
+      <c r="T20" t="b">
+        <v>1</v>
+      </c>
+      <c r="U20" t="n">
+        <v>80</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="n">
+        <v>240</v>
+      </c>
+      <c r="X20" t="n">
+        <v>400</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD20" t="n">
+        <v>8.10709708687815</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>239</v>
+      </c>
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.366953125</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-0.030703125</v>
+      </c>
+      <c r="F21" t="n">
+        <v>56.46762959981378</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.04904188826244745</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.001901142926734533</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.4202851782025427</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>15.17095625</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1.830200000000001</v>
+      </c>
+      <c r="P21" t="n">
+        <v>12.7908875</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>2</v>
+      </c>
+      <c r="R21" t="n">
+        <v>80828</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" t="b">
+        <v>1</v>
+      </c>
+      <c r="U21" t="n">
+        <v>77</v>
+      </c>
+      <c r="V21" t="n">
+        <v>10</v>
+      </c>
+      <c r="W21" t="n">
+        <v>240</v>
+      </c>
+      <c r="X21" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD21" t="n">
+        <v>1.54370905409459</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix some bugs to generate surface files;still buggy in angle calculation when dealing with non-cubic unitcell substrate
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_ctr.xlsx
+++ b/dump_files/temp_data_ctr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD21"/>
+  <dimension ref="A1:AD28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2500,6 +2500,678 @@
         <v>1.54370905409459</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>239</v>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.369921875</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.03078125</v>
+      </c>
+      <c r="F22" t="n">
+        <v>57.74231311258944</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.04928864760245783</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.001907359417408593</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.437142534032867</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>15.1720875</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1.905537500000001</v>
+      </c>
+      <c r="P22" t="n">
+        <v>12.791425</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>2</v>
+      </c>
+      <c r="R22" t="n">
+        <v>80783</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1</v>
+      </c>
+      <c r="T22" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" t="n">
+        <v>77</v>
+      </c>
+      <c r="V22" t="n">
+        <v>10</v>
+      </c>
+      <c r="W22" t="n">
+        <v>240</v>
+      </c>
+      <c r="X22" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD22" t="n">
+        <v>1.567242433984148</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>239</v>
+      </c>
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.378671875</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.029140625</v>
+      </c>
+      <c r="F23" t="n">
+        <v>59.00248231300491</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.04955877145819353</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.001911389520358967</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.4540006788732852</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>15.1737125</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1.980875000000001</v>
+      </c>
+      <c r="P23" t="n">
+        <v>12.79205</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>2</v>
+      </c>
+      <c r="R23" t="n">
+        <v>80520</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1</v>
+      </c>
+      <c r="T23" t="b">
+        <v>1</v>
+      </c>
+      <c r="U23" t="n">
+        <v>77</v>
+      </c>
+      <c r="V23" t="n">
+        <v>10</v>
+      </c>
+      <c r="W23" t="n">
+        <v>240</v>
+      </c>
+      <c r="X23" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD23" t="n">
+        <v>1.629682359345268</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>239</v>
+      </c>
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.365078125</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.032890625</v>
+      </c>
+      <c r="F24" t="n">
+        <v>60.0986020400894</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0497999872003506</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.001916193157425531</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.4708585412821902</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>15.17575625</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2.056212500000001</v>
+      </c>
+      <c r="P24" t="n">
+        <v>12.79265</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>2</v>
+      </c>
+      <c r="R24" t="n">
+        <v>80388</v>
+      </c>
+      <c r="S24" t="n">
+        <v>1</v>
+      </c>
+      <c r="T24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U24" t="n">
+        <v>77</v>
+      </c>
+      <c r="V24" t="n">
+        <v>10</v>
+      </c>
+      <c r="W24" t="n">
+        <v>240</v>
+      </c>
+      <c r="X24" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD24" t="n">
+        <v>1.646271365061731</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>239</v>
+      </c>
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.3721875</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-0.0309375</v>
+      </c>
+      <c r="F25" t="n">
+        <v>61.43230919474978</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.05000641473902703</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.001916285444844785</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.4877137686888458</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>15.17824375</v>
+      </c>
+      <c r="O25" t="n">
+        <v>2.1315375</v>
+      </c>
+      <c r="P25" t="n">
+        <v>12.7932375</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>2</v>
+      </c>
+      <c r="R25" t="n">
+        <v>80277</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
+      </c>
+      <c r="T25" t="b">
+        <v>1</v>
+      </c>
+      <c r="U25" t="n">
+        <v>77</v>
+      </c>
+      <c r="V25" t="n">
+        <v>10</v>
+      </c>
+      <c r="W25" t="n">
+        <v>240</v>
+      </c>
+      <c r="X25" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD25" t="n">
+        <v>1.690213258276134</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>239</v>
+      </c>
+      <c r="C26" t="n">
+        <v>24</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.3696875</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-0.03078125</v>
+      </c>
+      <c r="F26" t="n">
+        <v>62.73743421508154</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.05010663951524311</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.001915920986484906</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.5045701660188114</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>15.181175</v>
+      </c>
+      <c r="O26" t="n">
+        <v>2.206875</v>
+      </c>
+      <c r="P26" t="n">
+        <v>12.793825</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>2</v>
+      </c>
+      <c r="R26" t="n">
+        <v>80491</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1</v>
+      </c>
+      <c r="T26" t="b">
+        <v>1</v>
+      </c>
+      <c r="U26" t="n">
+        <v>77</v>
+      </c>
+      <c r="V26" t="n">
+        <v>10</v>
+      </c>
+      <c r="W26" t="n">
+        <v>240</v>
+      </c>
+      <c r="X26" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD26" t="n">
+        <v>1.696000534247075</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>239</v>
+      </c>
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.37265625</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-0.031328125</v>
+      </c>
+      <c r="F27" t="n">
+        <v>63.90097069853066</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.05033477273181355</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.001923591010199174</v>
+      </c>
+      <c r="I27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.5214279424411044</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>15.1845875</v>
+      </c>
+      <c r="O27" t="n">
+        <v>2.2822125</v>
+      </c>
+      <c r="P27" t="n">
+        <v>12.7945</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>2</v>
+      </c>
+      <c r="R27" t="n">
+        <v>80448</v>
+      </c>
+      <c r="S27" t="n">
+        <v>1</v>
+      </c>
+      <c r="T27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U27" t="n">
+        <v>77</v>
+      </c>
+      <c r="V27" t="n">
+        <v>10</v>
+      </c>
+      <c r="W27" t="n">
+        <v>240</v>
+      </c>
+      <c r="X27" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD27" t="n">
+        <v>1.762057682353713</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>239</v>
+      </c>
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.37125</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.03046875</v>
+      </c>
+      <c r="F28" t="n">
+        <v>64.71992978692553</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.05044477057173122</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.00192518646410966</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.538285347725167</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>15.1884375</v>
+      </c>
+      <c r="O28" t="n">
+        <v>2.35755</v>
+      </c>
+      <c r="P28" t="n">
+        <v>12.7951625</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>2</v>
+      </c>
+      <c r="R28" t="n">
+        <v>80492</v>
+      </c>
+      <c r="S28" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" t="b">
+        <v>1</v>
+      </c>
+      <c r="U28" t="n">
+        <v>77</v>
+      </c>
+      <c r="V28" t="n">
+        <v>10</v>
+      </c>
+      <c r="W28" t="n">
+        <v>240</v>
+      </c>
+      <c r="X28" t="n">
+        <v>302</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AB28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AD28" t="n">
+        <v>1.751368406321544</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
remove the fluctuation component from the error bar evaluation, now error bar is possoin error purely.
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_ctr.xlsx
+++ b/dump_files/temp_data_ctr.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG51"/>
+  <dimension ref="A1:AG72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,13 +613,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0764797415591887</v>
+        <v>0.09721576304624097</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03905993799005809</v>
+        <v>0.04125126191330538</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0002612929208226675</v>
+        <v>0.0002542914692872765</v>
       </c>
       <c r="I2" t="n">
         <v>2</v>
@@ -658,13 +658,13 @@
         <v>1</v>
       </c>
       <c r="U2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
         <v>120</v>
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="AE2" t="n">
-        <v>0.04816585102283663</v>
+        <v>0.1135486862779087</v>
       </c>
       <c r="AF2" t="n">
         <v>0.0001589856854948248</v>
@@ -718,13 +718,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F3" t="n">
-        <v>0.399831418744742</v>
+        <v>0.3604410818283874</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04571072931874342</v>
+        <v>0.05300394812593208</v>
       </c>
       <c r="H3" t="n">
-        <v>0.000281470490348347</v>
+        <v>0.0002772119912235288</v>
       </c>
       <c r="I3" t="n">
         <v>2</v>
@@ -766,10 +766,10 @@
         <v>1</v>
       </c>
       <c r="V3" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
         <v>120</v>
@@ -797,13 +797,13 @@
         </is>
       </c>
       <c r="AE3" t="n">
-        <v>0.05312430390324365</v>
+        <v>0.1680814628053406</v>
       </c>
       <c r="AF3" t="n">
         <v>0.0001335700357694114</v>
       </c>
       <c r="AG3" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -823,13 +823,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F4" t="n">
-        <v>0.599816633813235</v>
+        <v>0.5016013013753848</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04396393891469768</v>
+        <v>0.04900457046083301</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0002919527519200722</v>
+        <v>0.0002878072665654365</v>
       </c>
       <c r="I4" t="n">
         <v>2</v>
@@ -871,10 +871,10 @@
         <v>1</v>
       </c>
       <c r="V4" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
         <v>120</v>
@@ -898,17 +898,17 @@
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE4" t="n">
-        <v>0.05316468084068966</v>
+        <v>0.2077176018045037</v>
       </c>
       <c r="AF4" t="n">
         <v>0.0004261338930113039</v>
       </c>
       <c r="AG4" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -928,13 +928,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5569871463927891</v>
+        <v>0.4685319849791202</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04478417334253781</v>
+        <v>0.05433813830395584</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000296960457833451</v>
+        <v>0.0002923564553438407</v>
       </c>
       <c r="I5" t="n">
         <v>2</v>
@@ -976,10 +976,10 @@
         <v>1</v>
       </c>
       <c r="V5" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
         <v>120</v>
@@ -1003,17 +1003,17 @@
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE5" t="n">
-        <v>0.05689482210575092</v>
+        <v>0.2181693134248116</v>
       </c>
       <c r="AF5" t="n">
         <v>0.000718676592156832</v>
       </c>
       <c r="AG5" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1033,13 +1033,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3772420998557531</v>
+        <v>0.3231612215533674</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04546355675638912</v>
+        <v>0.04710827659715244</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0002955654443918182</v>
+        <v>0.0002897783946061783</v>
       </c>
       <c r="I6" t="n">
         <v>2</v>
@@ -1081,10 +1081,10 @@
         <v>1</v>
       </c>
       <c r="V6" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
         <v>120</v>
@@ -1108,17 +1108,17 @@
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE6" t="n">
-        <v>0.05396986467876685</v>
+        <v>0.189688000662597</v>
       </c>
       <c r="AF6" t="n">
         <v>0.001011189028630286</v>
       </c>
       <c r="AG6" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1138,13 +1138,13 @@
         <v>-0.001328125</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3002827235044237</v>
+        <v>0.2358807239767866</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04576081504304744</v>
+        <v>0.05373298183579019</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0002922942740059807</v>
+        <v>0.0002867624075509777</v>
       </c>
       <c r="I7" t="n">
         <v>2</v>
@@ -1186,10 +1186,10 @@
         <v>1</v>
       </c>
       <c r="V7" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
         <v>120</v>
@@ -1213,17 +1213,17 @@
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE7" t="n">
-        <v>0.06020876104209855</v>
+        <v>0.1620931418455959</v>
       </c>
       <c r="AF7" t="n">
         <v>0.001303701231108943</v>
       </c>
       <c r="AG7" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1243,13 +1243,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1881732894607532</v>
+        <v>0.1752532632878965</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04469348111190367</v>
+        <v>0.05666028735649346</v>
       </c>
       <c r="H8" t="n">
-        <v>0.000289739556215312</v>
+        <v>0.0002824059200833066</v>
       </c>
       <c r="I8" t="n">
         <v>2</v>
@@ -1291,10 +1291,10 @@
         <v>1</v>
       </c>
       <c r="V8" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
         <v>120</v>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE8" t="n">
-        <v>0.05381840219155518</v>
+        <v>0.1502211440096811</v>
       </c>
       <c r="AF8" t="n">
         <v>0.001596208987665999</v>
       </c>
       <c r="AG8" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1348,13 +1348,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1597779954669115</v>
+        <v>0.1601861918720787</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0437302971516045</v>
+        <v>0.04852358814720904</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0002872701971481161</v>
+        <v>0.0002798863829567043</v>
       </c>
       <c r="I9" t="n">
         <v>2</v>
@@ -1396,10 +1396,10 @@
         <v>1</v>
       </c>
       <c r="V9" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
         <v>120</v>
@@ -1423,17 +1423,17 @@
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE9" t="n">
-        <v>0.05443422729192952</v>
+        <v>0.1311107407624554</v>
       </c>
       <c r="AF9" t="n">
         <v>0.001888642857126413</v>
       </c>
       <c r="AG9" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1453,13 +1453,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1026389804468619</v>
+        <v>0.1246096315346143</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04190559006113124</v>
+        <v>0.05296435373276343</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0002838189930593808</v>
+        <v>0.0002757035486516593</v>
       </c>
       <c r="I10" t="n">
         <v>2</v>
@@ -1501,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="V10" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
         <v>120</v>
@@ -1528,17 +1528,17 @@
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE10" t="n">
-        <v>0.05260824480494995</v>
+        <v>0.1280802061283253</v>
       </c>
       <c r="AF10" t="n">
         <v>0.002181063517051033</v>
       </c>
       <c r="AG10" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1558,13 +1558,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1056745592008538</v>
+        <v>0.1221997738995097</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0543336859646028</v>
+        <v>0.05700488559693473</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0002840198195205669</v>
+        <v>0.000275556539765143</v>
       </c>
       <c r="I11" t="n">
         <v>2</v>
@@ -1606,10 +1606,10 @@
         <v>1</v>
       </c>
       <c r="V11" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X11" t="n">
         <v>120</v>
@@ -1633,17 +1633,17 @@
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE11" t="n">
-        <v>0.06208450450453818</v>
+        <v>0.1366536523978645</v>
       </c>
       <c r="AF11" t="n">
         <v>0.002473415448778893</v>
       </c>
       <c r="AG11" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1663,13 +1663,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06997865568079911</v>
+        <v>0.09074415077719829</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0407540750822448</v>
+        <v>0.04083701844053463</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0002833164998113166</v>
+        <v>0.0002756911609827324</v>
       </c>
       <c r="I12" t="n">
         <v>2</v>
@@ -1711,10 +1711,10 @@
         <v>1</v>
       </c>
       <c r="V12" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W12" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X12" t="n">
         <v>120</v>
@@ -1738,17 +1738,17 @@
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE12" t="n">
-        <v>0.0478560462372914</v>
+        <v>0.1219435255325556</v>
       </c>
       <c r="AF12" t="n">
         <v>0.002765730954260923</v>
       </c>
       <c r="AG12" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1768,13 +1768,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F13" t="n">
-        <v>0.06120684231986191</v>
+        <v>0.1057960615614632</v>
       </c>
       <c r="G13" t="n">
-        <v>0.04537322521821108</v>
+        <v>0.05055945498855801</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0002818533354045538</v>
+        <v>0.0002723328105967581</v>
       </c>
       <c r="I13" t="n">
         <v>2</v>
@@ -1816,10 +1816,10 @@
         <v>1</v>
       </c>
       <c r="V13" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X13" t="n">
         <v>120</v>
@@ -1843,17 +1843,17 @@
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE13" t="n">
-        <v>0.05336100036159234</v>
+        <v>0.120808160117275</v>
       </c>
       <c r="AF13" t="n">
         <v>0.003058037269159208</v>
       </c>
       <c r="AG13" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1873,13 +1873,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0749864695639202</v>
+        <v>0.08203446122634632</v>
       </c>
       <c r="G14" t="n">
-        <v>0.04474936832110227</v>
+        <v>0.04782319831993857</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0002759921267635059</v>
+        <v>0.0002685630121605095</v>
       </c>
       <c r="I14" t="n">
         <v>2</v>
@@ -1921,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="V14" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X14" t="n">
         <v>120</v>
@@ -1948,17 +1948,17 @@
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE14" t="n">
-        <v>0.05538014769721993</v>
+        <v>0.1156694581905917</v>
       </c>
       <c r="AF14" t="n">
         <v>0.003350170867517325</v>
       </c>
       <c r="AG14" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1978,13 +1978,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F15" t="n">
-        <v>0.06112716556812643</v>
+        <v>0.08663175493770531</v>
       </c>
       <c r="G15" t="n">
-        <v>0.04984537077028776</v>
+        <v>0.04755060219320809</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0002761792763880951</v>
+        <v>0.0002680029845205473</v>
       </c>
       <c r="I15" t="n">
         <v>2</v>
@@ -2026,10 +2026,10 @@
         <v>1</v>
       </c>
       <c r="V15" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X15" t="n">
         <v>120</v>
@@ -2053,17 +2053,17 @@
       </c>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE15" t="n">
-        <v>0.05547676954839642</v>
+        <v>0.1201554965591009</v>
       </c>
       <c r="AF15" t="n">
         <v>0.003642322582859247</v>
       </c>
       <c r="AG15" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2083,13 +2083,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F16" t="n">
-        <v>0.09193848102884131</v>
+        <v>0.08195919090109033</v>
       </c>
       <c r="G16" t="n">
-        <v>0.04587065448188608</v>
+        <v>0.04690142569321648</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0002776670347874103</v>
+        <v>0.0002696380146021228</v>
       </c>
       <c r="I16" t="n">
         <v>2</v>
@@ -2131,10 +2131,10 @@
         <v>1</v>
       </c>
       <c r="V16" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X16" t="n">
         <v>120</v>
@@ -2158,17 +2158,17 @@
       </c>
       <c r="AD16" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE16" t="n">
-        <v>0.05199340441562435</v>
+        <v>0.119972380598467</v>
       </c>
       <c r="AF16" t="n">
         <v>0.003934380251146528</v>
       </c>
       <c r="AG16" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2188,13 +2188,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F17" t="n">
-        <v>0.05579762320267311</v>
+        <v>0.07322718014511045</v>
       </c>
       <c r="G17" t="n">
-        <v>0.04914812464050251</v>
+        <v>0.05390076501814485</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0002767376737123554</v>
+        <v>0.0002665056537893042</v>
       </c>
       <c r="I17" t="n">
         <v>2</v>
@@ -2236,10 +2236,10 @@
         <v>1</v>
       </c>
       <c r="V17" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X17" t="n">
         <v>120</v>
@@ -2263,17 +2263,17 @@
       </c>
       <c r="AD17" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE17" t="n">
-        <v>0.05373885454066227</v>
+        <v>0.1270999661326299</v>
       </c>
       <c r="AF17" t="n">
         <v>0.004226326624840558</v>
       </c>
       <c r="AG17" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2293,13 +2293,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F18" t="n">
-        <v>0.08267578616106608</v>
+        <v>0.08736425290719792</v>
       </c>
       <c r="G18" t="n">
-        <v>0.04814656832547622</v>
+        <v>0.04868541168932768</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0002790801120946578</v>
+        <v>0.0002695757899263082</v>
       </c>
       <c r="I18" t="n">
         <v>2</v>
@@ -2341,10 +2341,10 @@
         <v>1</v>
       </c>
       <c r="V18" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X18" t="n">
         <v>120</v>
@@ -2368,17 +2368,17 @@
       </c>
       <c r="AD18" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE18" t="n">
-        <v>0.0529665028670006</v>
+        <v>0.1210828679212608</v>
       </c>
       <c r="AF18" t="n">
         <v>0.004518227805618716</v>
       </c>
       <c r="AG18" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2398,13 +2398,13 @@
         <v>-0.00078125</v>
       </c>
       <c r="F19" t="n">
-        <v>0.06052212184842062</v>
+        <v>0.08470383183684116</v>
       </c>
       <c r="G19" t="n">
-        <v>0.04960210360796548</v>
+        <v>0.04810355329359534</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0002793344717466512</v>
+        <v>0.0002700411257971357</v>
       </c>
       <c r="I19" t="n">
         <v>2</v>
@@ -2446,10 +2446,10 @@
         <v>1</v>
       </c>
       <c r="V19" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X19" t="n">
         <v>120</v>
@@ -2473,17 +2473,17 @@
       </c>
       <c r="AD19" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE19" t="n">
-        <v>0.05278842188031275</v>
+        <v>0.1245521005251173</v>
       </c>
       <c r="AF19" t="n">
         <v>0.004809998234665402</v>
       </c>
       <c r="AG19" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2503,13 +2503,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F20" t="n">
-        <v>0.07504126735524852</v>
+        <v>0.07920014823169345</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0442062671953949</v>
+        <v>0.04242965664545872</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0002793085951288387</v>
+        <v>0.000270289764482096</v>
       </c>
       <c r="I20" t="n">
         <v>2</v>
@@ -2551,10 +2551,10 @@
         <v>1</v>
       </c>
       <c r="V20" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X20" t="n">
         <v>120</v>
@@ -2578,17 +2578,17 @@
       </c>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE20" t="n">
-        <v>0.04957167503171273</v>
+        <v>0.1202735761534576</v>
       </c>
       <c r="AF20" t="n">
         <v>0.005101681710295304</v>
       </c>
       <c r="AG20" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2608,13 +2608,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0846648792895075</v>
+        <v>0.06683118177761183</v>
       </c>
       <c r="G21" t="n">
-        <v>0.05090547075718926</v>
+        <v>0.05109813028974211</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0002817320319629621</v>
+        <v>0.0002726237377671927</v>
       </c>
       <c r="I21" t="n">
         <v>2</v>
@@ -2656,10 +2656,10 @@
         <v>1</v>
       </c>
       <c r="V21" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X21" t="n">
         <v>120</v>
@@ -2683,17 +2683,17 @@
       </c>
       <c r="AD21" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE21" t="n">
-        <v>0.06114476105219446</v>
+        <v>0.1177386044058978</v>
       </c>
       <c r="AF21" t="n">
         <v>0.005393211541889114</v>
       </c>
       <c r="AG21" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2713,13 +2713,13 @@
         <v>-0.000625</v>
       </c>
       <c r="F22" t="n">
-        <v>0.04278590211031193</v>
+        <v>0.09290391057144712</v>
       </c>
       <c r="G22" t="n">
-        <v>0.04823521024484088</v>
+        <v>0.05097844912617895</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0002845787968767183</v>
+        <v>0.0002730219827217517</v>
       </c>
       <c r="I22" t="n">
         <v>2</v>
@@ -2761,10 +2761,10 @@
         <v>1</v>
       </c>
       <c r="V22" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X22" t="n">
         <v>120</v>
@@ -2788,17 +2788,17 @@
       </c>
       <c r="AD22" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE22" t="n">
-        <v>0.05350768904129741</v>
+        <v>0.1228401522303609</v>
       </c>
       <c r="AF22" t="n">
         <v>0.00568460021300261</v>
       </c>
       <c r="AG22" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2818,13 +2818,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F23" t="n">
-        <v>0.05567512197711777</v>
+        <v>0.08291801776632363</v>
       </c>
       <c r="G23" t="n">
-        <v>0.04305159256625588</v>
+        <v>0.04953594261343068</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0002839989594979024</v>
+        <v>0.0002748825745416441</v>
       </c>
       <c r="I23" t="n">
         <v>2</v>
@@ -2866,10 +2866,10 @@
         <v>1</v>
       </c>
       <c r="V23" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W23" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X23" t="n">
         <v>120</v>
@@ -2893,17 +2893,17 @@
       </c>
       <c r="AD23" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE23" t="n">
-        <v>0.04906083071874569</v>
+        <v>0.1204788081583832</v>
       </c>
       <c r="AF23" t="n">
         <v>0.005975866688449988</v>
       </c>
       <c r="AG23" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2923,13 +2923,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0614374806498119</v>
+        <v>0.0797304057180388</v>
       </c>
       <c r="G24" t="n">
-        <v>0.04579738428813349</v>
+        <v>0.04519338705769702</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0002859362686881916</v>
+        <v>0.00027648287709666</v>
       </c>
       <c r="I24" t="n">
         <v>2</v>
@@ -2971,10 +2971,10 @@
         <v>1</v>
       </c>
       <c r="V24" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X24" t="n">
         <v>120</v>
@@ -2998,17 +2998,17 @@
       </c>
       <c r="AD24" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE24" t="n">
-        <v>0.05065156510076754</v>
+        <v>0.1191963502624022</v>
       </c>
       <c r="AF24" t="n">
         <v>0.00626699700686289</v>
       </c>
       <c r="AG24" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -3028,13 +3028,13 @@
         <v>-0.001328125</v>
       </c>
       <c r="F25" t="n">
-        <v>0.09175258444842178</v>
+        <v>0.09698035612846154</v>
       </c>
       <c r="G25" t="n">
-        <v>0.05187140150281065</v>
+        <v>0.04950623461935742</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00028743107201662</v>
+        <v>0.0002787711020005231</v>
       </c>
       <c r="I25" t="n">
         <v>2</v>
@@ -3076,10 +3076,10 @@
         <v>1</v>
       </c>
       <c r="V25" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X25" t="n">
         <v>120</v>
@@ -3103,17 +3103,17 @@
       </c>
       <c r="AD25" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE25" t="n">
-        <v>0.05709129064325553</v>
+        <v>0.1239146219275478</v>
       </c>
       <c r="AF25" t="n">
         <v>0.006557980366834047</v>
       </c>
       <c r="AG25" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -3133,13 +3133,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F26" t="n">
-        <v>0.07614108208945902</v>
+        <v>0.1030441389734955</v>
       </c>
       <c r="G26" t="n">
-        <v>0.05272978068735744</v>
+        <v>0.05207773457660346</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0002881640091617848</v>
+        <v>0.0002788508126679293</v>
       </c>
       <c r="I26" t="n">
         <v>2</v>
@@ -3181,10 +3181,10 @@
         <v>1</v>
       </c>
       <c r="V26" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W26" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X26" t="n">
         <v>120</v>
@@ -3208,17 +3208,17 @@
       </c>
       <c r="AD26" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE26" t="n">
-        <v>0.05794953013637844</v>
+        <v>0.1303840863383617</v>
       </c>
       <c r="AF26" t="n">
         <v>0.006848785725417059</v>
       </c>
       <c r="AG26" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3238,13 +3238,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0699469496304809</v>
+        <v>0.1050006387663884</v>
       </c>
       <c r="G27" t="n">
-        <v>0.04608051273250414</v>
+        <v>0.04532653348932794</v>
       </c>
       <c r="H27" t="n">
-        <v>0.000291018583004455</v>
+        <v>0.0002813773213401774</v>
       </c>
       <c r="I27" t="n">
         <v>2</v>
@@ -3286,10 +3286,10 @@
         <v>1</v>
       </c>
       <c r="V27" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W27" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X27" t="n">
         <v>120</v>
@@ -3313,17 +3313,17 @@
       </c>
       <c r="AD27" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE27" t="n">
-        <v>0.05128638810186835</v>
+        <v>0.1228113526480281</v>
       </c>
       <c r="AF27" t="n">
         <v>0.007139343835434949</v>
       </c>
       <c r="AG27" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -3343,13 +3343,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1057561716042622</v>
+        <v>0.1225949607956582</v>
       </c>
       <c r="G28" t="n">
-        <v>0.04884906987823098</v>
+        <v>0.05041989973010523</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0002917339617873584</v>
+        <v>0.000282646221157708</v>
       </c>
       <c r="I28" t="n">
         <v>2</v>
@@ -3391,10 +3391,10 @@
         <v>1</v>
       </c>
       <c r="V28" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W28" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X28" t="n">
         <v>120</v>
@@ -3418,17 +3418,17 @@
       </c>
       <c r="AD28" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE28" t="n">
-        <v>0.05129928500317994</v>
+        <v>0.1200837056351705</v>
       </c>
       <c r="AF28" t="n">
         <v>0.007429672231614669</v>
       </c>
       <c r="AG28" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -3448,13 +3448,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1301760763767931</v>
+        <v>0.1448867105225271</v>
       </c>
       <c r="G29" t="n">
-        <v>0.05049656513847391</v>
+        <v>0.05363487925179018</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0002957401696222051</v>
+        <v>0.0002866603027744123</v>
       </c>
       <c r="I29" t="n">
         <v>2</v>
@@ -3496,10 +3496,10 @@
         <v>1</v>
       </c>
       <c r="V29" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X29" t="n">
         <v>120</v>
@@ -3523,17 +3523,17 @@
       </c>
       <c r="AD29" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE29" t="n">
-        <v>0.05614772828898582</v>
+        <v>0.1319899305828813</v>
       </c>
       <c r="AF29" t="n">
         <v>0.007719861208897987</v>
       </c>
       <c r="AG29" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -3553,13 +3553,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1506422257740953</v>
+        <v>0.1533770012101666</v>
       </c>
       <c r="G30" t="n">
-        <v>0.04838744053188498</v>
+        <v>0.05833109459423275</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0002978278319002485</v>
+        <v>0.0002888893775793694</v>
       </c>
       <c r="I30" t="n">
         <v>2</v>
@@ -3601,10 +3601,10 @@
         <v>1</v>
       </c>
       <c r="V30" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W30" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X30" t="n">
         <v>120</v>
@@ -3628,17 +3628,17 @@
       </c>
       <c r="AD30" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE30" t="n">
-        <v>0.05974915310211178</v>
+        <v>0.1393186496324103</v>
       </c>
       <c r="AF30" t="n">
         <v>0.008009747283939044</v>
       </c>
       <c r="AG30" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -3658,13 +3658,13 @@
         <v>-0.00078125</v>
       </c>
       <c r="F31" t="n">
-        <v>0.1878856510973284</v>
+        <v>0.2156825297948096</v>
       </c>
       <c r="G31" t="n">
-        <v>0.05288908111508341</v>
+        <v>0.05835090590493049</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0003013296670597441</v>
+        <v>0.0002915520190832356</v>
       </c>
       <c r="I31" t="n">
         <v>2</v>
@@ -3706,10 +3706,10 @@
         <v>1</v>
       </c>
       <c r="V31" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W31" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X31" t="n">
         <v>120</v>
@@ -3733,17 +3733,17 @@
       </c>
       <c r="AD31" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE31" t="n">
-        <v>0.05724098132536806</v>
+        <v>0.1491751557320692</v>
       </c>
       <c r="AF31" t="n">
         <v>0.008299456036458841</v>
       </c>
       <c r="AG31" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -3763,13 +3763,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F32" t="n">
-        <v>0.2714546717412984</v>
+        <v>0.2590556930059474</v>
       </c>
       <c r="G32" t="n">
-        <v>0.05086939343929461</v>
+        <v>0.05844727028015451</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0003088533963222146</v>
+        <v>0.0002997184141911398</v>
       </c>
       <c r="I32" t="n">
         <v>2</v>
@@ -3811,10 +3811,10 @@
         <v>1</v>
       </c>
       <c r="V32" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W32" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X32" t="n">
         <v>120</v>
@@ -3838,17 +3838,17 @@
       </c>
       <c r="AD32" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE32" t="n">
-        <v>0.05830402631985099</v>
+        <v>0.1532164466467745</v>
       </c>
       <c r="AF32" t="n">
         <v>0.00858879184594641</v>
       </c>
       <c r="AG32" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -3868,13 +3868,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3822215894979859</v>
+        <v>0.3555168969006461</v>
       </c>
       <c r="G33" t="n">
-        <v>0.05552981266430723</v>
+        <v>0.05887445548708479</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0003220019958973222</v>
+        <v>0.0003116433503970234</v>
       </c>
       <c r="I33" t="n">
         <v>2</v>
@@ -3916,10 +3916,10 @@
         <v>1</v>
       </c>
       <c r="V33" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="W33" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X33" t="n">
         <v>120</v>
@@ -3943,17 +3943,17 @@
       </c>
       <c r="AD33" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE33" t="n">
-        <v>0.06495350823628604</v>
+        <v>0.1738163247503492</v>
       </c>
       <c r="AF33" t="n">
         <v>0.008877879897123431</v>
       </c>
       <c r="AG33" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -3973,13 +3973,13 @@
         <v>-0.000703125</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5662365886528147</v>
+        <v>0.6172586911667445</v>
       </c>
       <c r="G34" t="n">
-        <v>0.05084154582544288</v>
+        <v>0.04874590225026868</v>
       </c>
       <c r="H34" t="n">
-        <v>0.000341185393628949</v>
+        <v>0.0003232404613713097</v>
       </c>
       <c r="I34" t="n">
         <v>2</v>
@@ -4021,16 +4021,16 @@
         <v>1</v>
       </c>
       <c r="V34" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W34" t="n">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="X34" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y34" t="n">
-        <v>400</v>
+        <v>246</v>
       </c>
       <c r="Z34" t="n">
         <v>2</v>
@@ -4048,17 +4048,17 @@
       </c>
       <c r="AD34" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE34" t="n">
-        <v>0.05960791307720424</v>
+        <v>0.1269478988909661</v>
       </c>
       <c r="AF34" t="n">
         <v>0.009166711083625869</v>
       </c>
       <c r="AG34" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -4078,13 +4078,13 @@
         <v>-0.00078125</v>
       </c>
       <c r="F35" t="n">
-        <v>1.02744722726985</v>
+        <v>1.111434321943296</v>
       </c>
       <c r="G35" t="n">
-        <v>0.06605933374259081</v>
+        <v>0.06654292622874805</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0003982237065797988</v>
+        <v>0.0003624299259517576</v>
       </c>
       <c r="I35" t="n">
         <v>2</v>
@@ -4126,16 +4126,16 @@
         <v>1</v>
       </c>
       <c r="V35" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W35" t="n">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="X35" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y35" t="n">
-        <v>400</v>
+        <v>246</v>
       </c>
       <c r="Z35" t="n">
         <v>2</v>
@@ -4153,17 +4153,17 @@
       </c>
       <c r="AD35" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE35" t="n">
-        <v>0.08721292245745318</v>
+        <v>0.1547283019047085</v>
       </c>
       <c r="AF35" t="n">
         <v>0.00945514894295787</v>
       </c>
       <c r="AG35" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -4183,13 +4183,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F36" t="n">
-        <v>2.466271835178299</v>
+        <v>2.630499140860354</v>
       </c>
       <c r="G36" t="n">
-        <v>0.07957380218535742</v>
+        <v>0.1025161056027936</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0005328021978021978</v>
+        <v>0.0004760663281195381</v>
       </c>
       <c r="I36" t="n">
         <v>2</v>
@@ -4231,16 +4231,16 @@
         <v>1</v>
       </c>
       <c r="V36" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W36" t="n">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="X36" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y36" t="n">
-        <v>192</v>
+        <v>246</v>
       </c>
       <c r="Z36" t="n">
         <v>2</v>
@@ -4258,17 +4258,17 @@
       </c>
       <c r="AD36" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE36" t="n">
-        <v>0.1142795049896475</v>
+        <v>0.2206179964242447</v>
       </c>
       <c r="AF36" t="n">
         <v>0.009743266832289132</v>
       </c>
       <c r="AG36" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -4288,13 +4288,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F37" t="n">
-        <v>9.137278134643649</v>
+        <v>316.313201947379</v>
       </c>
       <c r="G37" t="n">
-        <v>0.5762358470695149</v>
+        <v>21.18288167517701</v>
       </c>
       <c r="H37" t="n">
-        <v>0.0009698214036196458</v>
+        <v>0.002150355785928223</v>
       </c>
       <c r="I37" t="n">
         <v>2</v>
@@ -4336,16 +4336,16 @@
         <v>1</v>
       </c>
       <c r="V37" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W37" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X37" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y37" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z37" t="n">
         <v>2</v>
@@ -4363,17 +4363,17 @@
       </c>
       <c r="AD37" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE37" t="n">
-        <v>0.7769337422124647</v>
+        <v>29.7557562069466</v>
       </c>
       <c r="AF37" t="n">
         <v>0.0100309779327597</v>
       </c>
       <c r="AG37" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -4393,13 +4393,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F38" t="n">
-        <v>95910.33108163434</v>
+        <v>95749.02476473671</v>
       </c>
       <c r="G38" t="n">
-        <v>244.3193372937309</v>
+        <v>222.6536155149417</v>
       </c>
       <c r="H38" t="n">
-        <v>0.2959681001938033</v>
+        <v>0.07145634533579684</v>
       </c>
       <c r="I38" t="n">
         <v>2</v>
@@ -4438,19 +4438,19 @@
         <v>3.697421966131398e-05</v>
       </c>
       <c r="U38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V38" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W38" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X38" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y38" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z38" t="n">
         <v>2</v>
@@ -4468,17 +4468,17 @@
       </c>
       <c r="AD38" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE38" t="n">
-        <v>237.8111222685276</v>
+        <v>317.9313402897287</v>
       </c>
       <c r="AF38" t="n">
         <v>0.01031832868477658</v>
       </c>
       <c r="AG38" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -4498,13 +4498,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F39" t="n">
-        <v>10.48950920896432</v>
+        <v>-384.2689460127888</v>
       </c>
       <c r="G39" t="n">
-        <v>0.3409672920650652</v>
+        <v>119.6966770668493</v>
       </c>
       <c r="H39" t="n">
-        <v>0.001953075338975339</v>
+        <v>0.1706639802868804</v>
       </c>
       <c r="I39" t="n">
         <v>2</v>
@@ -4546,16 +4546,16 @@
         <v>1</v>
       </c>
       <c r="V39" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W39" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X39" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y39" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z39" t="n">
         <v>2</v>
@@ -4573,17 +4573,17 @@
       </c>
       <c r="AD39" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE39" t="n">
-        <v>0.6100091554823772</v>
+        <v>1337.640143581306</v>
       </c>
       <c r="AF39" t="n">
         <v>0.01060528634485899</v>
       </c>
       <c r="AG39" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -4603,13 +4603,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F40" t="n">
-        <v>1.839224460880482</v>
+        <v>1.996909137288126</v>
       </c>
       <c r="G40" t="n">
-        <v>0.08528241636981106</v>
+        <v>0.1548786210945777</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0006429306249889636</v>
+        <v>0.0006924308808424569</v>
       </c>
       <c r="I40" t="n">
         <v>2</v>
@@ -4651,16 +4651,16 @@
         <v>1</v>
       </c>
       <c r="V40" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W40" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X40" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y40" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z40" t="n">
         <v>2</v>
@@ -4678,17 +4678,17 @@
       </c>
       <c r="AD40" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE40" t="n">
-        <v>0.1145803493708675</v>
+        <v>0.285170065257351</v>
       </c>
       <c r="AF40" t="n">
         <v>0.01089177415282423</v>
       </c>
       <c r="AG40" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -4708,13 +4708,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F41" t="n">
-        <v>0.6084867007472529</v>
+        <v>0.7370613716013223</v>
       </c>
       <c r="G41" t="n">
-        <v>0.03024718574570079</v>
+        <v>0.0545397458742878</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0004132163579512347</v>
+        <v>0.0003947367777762825</v>
       </c>
       <c r="I41" t="n">
         <v>2</v>
@@ -4756,16 +4756,16 @@
         <v>1</v>
       </c>
       <c r="V41" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W41" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X41" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y41" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z41" t="n">
         <v>2</v>
@@ -4783,17 +4783,17 @@
       </c>
       <c r="AD41" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE41" t="n">
-        <v>0.03698693959718991</v>
+        <v>0.1320619435061224</v>
       </c>
       <c r="AF41" t="n">
         <v>0.01117777287134961</v>
       </c>
       <c r="AG41" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -4813,13 +4813,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F42" t="n">
-        <v>0.2936462848877062</v>
+        <v>0.3775148780549745</v>
       </c>
       <c r="G42" t="n">
-        <v>0.02134157667030225</v>
+        <v>0.03848275116261772</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0003463250110449015</v>
+        <v>0.0003263053903862362</v>
       </c>
       <c r="I42" t="n">
         <v>2</v>
@@ -4861,16 +4861,16 @@
         <v>1</v>
       </c>
       <c r="V42" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W42" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X42" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y42" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z42" t="n">
         <v>2</v>
@@ -4888,17 +4888,17 @@
       </c>
       <c r="AD42" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE42" t="n">
-        <v>0.03273246391847421</v>
+        <v>0.139589728584956</v>
       </c>
       <c r="AF42" t="n">
         <v>0.01146322545043837</v>
       </c>
       <c r="AG42" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -4918,13 +4918,13 @@
         <v>-0.001328125</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1734825538030717</v>
+        <v>0.2638764886905004</v>
       </c>
       <c r="G43" t="n">
-        <v>0.02930126466156225</v>
+        <v>0.04756878776761384</v>
       </c>
       <c r="H43" t="n">
-        <v>0.0003051253418055422</v>
+        <v>0.0002849796746712143</v>
       </c>
       <c r="I43" t="n">
         <v>2</v>
@@ -4966,16 +4966,16 @@
         <v>1</v>
       </c>
       <c r="V43" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W43" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X43" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y43" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z43" t="n">
         <v>2</v>
@@ -4993,17 +4993,17 @@
       </c>
       <c r="AD43" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE43" t="n">
-        <v>0.03478525618030711</v>
+        <v>0.1025487787046178</v>
       </c>
       <c r="AF43" t="n">
         <v>0.01174822448954057</v>
       </c>
       <c r="AG43" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -5023,13 +5023,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F44" t="n">
-        <v>0.1062819823181862</v>
+        <v>0.1568111503098943</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0277114581370771</v>
+        <v>0.03953048625817696</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0002842042632881104</v>
+        <v>0.0002659858962003597</v>
       </c>
       <c r="I44" t="n">
         <v>2</v>
@@ -5071,16 +5071,16 @@
         <v>1</v>
       </c>
       <c r="V44" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W44" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X44" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y44" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z44" t="n">
         <v>2</v>
@@ -5098,17 +5098,17 @@
       </c>
       <c r="AD44" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE44" t="n">
-        <v>0.03279684515484053</v>
+        <v>0.09544363380344689</v>
       </c>
       <c r="AF44" t="n">
         <v>0.0120326871026753</v>
       </c>
       <c r="AG44" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -5128,13 +5128,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F45" t="n">
-        <v>0.07879471194882627</v>
+        <v>0.1197117105036881</v>
       </c>
       <c r="G45" t="n">
-        <v>0.02852902059795393</v>
+        <v>0.03233753952337218</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0002649230072903446</v>
+        <v>0.0002536081811498539</v>
       </c>
       <c r="I45" t="n">
         <v>2</v>
@@ -5176,16 +5176,16 @@
         <v>1</v>
       </c>
       <c r="V45" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W45" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X45" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y45" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z45" t="n">
         <v>2</v>
@@ -5203,17 +5203,17 @@
       </c>
       <c r="AD45" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE45" t="n">
-        <v>0.02861710900718338</v>
+        <v>0.08672180578787174</v>
       </c>
       <c r="AF45" t="n">
         <v>0.01231645592062328</v>
       </c>
       <c r="AG45" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -5233,13 +5233,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F46" t="n">
-        <v>0.05221907815329555</v>
+        <v>0.0883551695782519</v>
       </c>
       <c r="G46" t="n">
-        <v>0.02181409160343193</v>
+        <v>0.03669597684540897</v>
       </c>
       <c r="H46" t="n">
-        <v>0.0002595577774607295</v>
+        <v>0.0002443933637556948</v>
       </c>
       <c r="I46" t="n">
         <v>2</v>
@@ -5281,16 +5281,16 @@
         <v>1</v>
       </c>
       <c r="V46" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W46" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X46" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y46" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z46" t="n">
         <v>2</v>
@@ -5308,17 +5308,17 @@
       </c>
       <c r="AD46" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE46" t="n">
-        <v>0.0265601798450627</v>
+        <v>0.08086283332728057</v>
       </c>
       <c r="AF46" t="n">
         <v>0.01259978099536829</v>
       </c>
       <c r="AG46" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -5338,13 +5338,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F47" t="n">
-        <v>0.05150658959888991</v>
+        <v>0.0793845045872507</v>
       </c>
       <c r="G47" t="n">
-        <v>0.02395616941140329</v>
+        <v>0.03572944954348665</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0002479499293350684</v>
+        <v>0.0002354932095634411</v>
       </c>
       <c r="I47" t="n">
         <v>2</v>
@@ -5386,16 +5386,16 @@
         <v>1</v>
       </c>
       <c r="V47" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W47" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X47" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y47" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z47" t="n">
         <v>2</v>
@@ -5413,17 +5413,17 @@
       </c>
       <c r="AD47" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE47" t="n">
-        <v>0.02652390799039291</v>
+        <v>0.08029166011482719</v>
       </c>
       <c r="AF47" t="n">
         <v>0.01288237003178895</v>
       </c>
       <c r="AG47" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -5443,13 +5443,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F48" t="n">
-        <v>0.05085398419726275</v>
+        <v>0.08581063411295586</v>
       </c>
       <c r="G48" t="n">
-        <v>0.02659649494611005</v>
+        <v>0.03817469781762103</v>
       </c>
       <c r="H48" t="n">
-        <v>0.0002418816070634208</v>
+        <v>0.0002303101608352863</v>
       </c>
       <c r="I48" t="n">
         <v>2</v>
@@ -5491,16 +5491,16 @@
         <v>1</v>
       </c>
       <c r="V48" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="W48" t="n">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="X48" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Y48" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z48" t="n">
         <v>2</v>
@@ -5518,17 +5518,17 @@
       </c>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE48" t="n">
-        <v>0.02755978230352253</v>
+        <v>0.07506196380497304</v>
       </c>
       <c r="AF48" t="n">
         <v>0.01316418543166263</v>
       </c>
       <c r="AG48" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -5548,13 +5548,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F49" t="n">
-        <v>0.03307278862684075</v>
+        <v>0.02123910526682641</v>
       </c>
       <c r="G49" t="n">
-        <v>0.02363109703054185</v>
+        <v>0.03250720381320851</v>
       </c>
       <c r="H49" t="n">
-        <v>0.0002387622428467559</v>
+        <v>0.0002383948795234443</v>
       </c>
       <c r="I49" t="n">
         <v>2</v>
@@ -5599,13 +5599,13 @@
         <v>65</v>
       </c>
       <c r="W49" t="n">
-        <v>151</v>
+        <v>86</v>
       </c>
       <c r="X49" t="n">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="Y49" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z49" t="n">
         <v>2</v>
@@ -5623,17 +5623,17 @@
       </c>
       <c r="AD49" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE49" t="n">
-        <v>0.0264407949459754</v>
+        <v>0.04206420724836923</v>
       </c>
       <c r="AF49" t="n">
         <v>0.01344538484793423</v>
       </c>
       <c r="AG49" t="n">
-        <v>-35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -5653,13 +5653,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F50" t="n">
-        <v>0.04376815902952562</v>
+        <v>0.01833779164974378</v>
       </c>
       <c r="G50" t="n">
-        <v>0.02554594282902289</v>
+        <v>0.02762915010094429</v>
       </c>
       <c r="H50" t="n">
-        <v>0.0002323684259662863</v>
+        <v>0.0002315635731333301</v>
       </c>
       <c r="I50" t="n">
         <v>2</v>
@@ -5704,13 +5704,13 @@
         <v>65</v>
       </c>
       <c r="W50" t="n">
-        <v>151</v>
+        <v>86</v>
       </c>
       <c r="X50" t="n">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="Y50" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z50" t="n">
         <v>2</v>
@@ -5728,17 +5728,17 @@
       </c>
       <c r="AD50" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE50" t="n">
-        <v>0.02826530708253469</v>
+        <v>0.0333947481170919</v>
       </c>
       <c r="AF50" t="n">
         <v>0.01372585148477921</v>
       </c>
       <c r="AG50" t="n">
-        <v>-35</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="51">
@@ -5758,13 +5758,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0264290900355694</v>
+        <v>0.02426505952039018</v>
       </c>
       <c r="G51" t="n">
-        <v>0.02231262667761866</v>
+        <v>0.03281341004002246</v>
       </c>
       <c r="H51" t="n">
-        <v>0.0002247420781923846</v>
+        <v>0.0002253089807492083</v>
       </c>
       <c r="I51" t="n">
         <v>2</v>
@@ -5809,13 +5809,13 @@
         <v>65</v>
       </c>
       <c r="W51" t="n">
-        <v>151</v>
+        <v>86</v>
       </c>
       <c r="X51" t="n">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="Y51" t="n">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="Z51" t="n">
         <v>2</v>
@@ -5833,17 +5833,2222 @@
       </c>
       <c r="AD51" t="inlineStr">
         <is>
-          <t>vincent</t>
+          <t>traditional</t>
         </is>
       </c>
       <c r="AE51" t="n">
-        <v>0.02563135950680018</v>
+        <v>0.0393174038424108</v>
       </c>
       <c r="AF51" t="n">
         <v>0.01400544596003308</v>
       </c>
       <c r="AG51" t="n">
-        <v>-35</v>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C52" t="n">
+        <v>50</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-0.586953125</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-0.0009375</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.01160003081164419</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.03448325044852299</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.0002267545053787523</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>2.69998821412326</v>
+      </c>
+      <c r="L52" t="n">
+        <v>40.093</v>
+      </c>
+      <c r="M52" t="n">
+        <v>90</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>24.0483875</v>
+      </c>
+      <c r="P52" t="n">
+        <v>17.932325</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" t="n">
+        <v>2</v>
+      </c>
+      <c r="S52" t="n">
+        <v>90584</v>
+      </c>
+      <c r="T52" t="n">
+        <v>1</v>
+      </c>
+      <c r="U52" t="b">
+        <v>1</v>
+      </c>
+      <c r="V52" t="n">
+        <v>65</v>
+      </c>
+      <c r="W52" t="n">
+        <v>86</v>
+      </c>
+      <c r="X52" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB52" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE52" t="n">
+        <v>0.04078864364124804</v>
+      </c>
+      <c r="AF52" t="n">
+        <v>0.01428418560140011</v>
+      </c>
+      <c r="AG52" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C53" t="n">
+        <v>51</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-0.585</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.0009375</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-0.004500512148603898</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.02756491697318644</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.0002246482979137438</v>
+      </c>
+      <c r="I53" t="n">
+        <v>2</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>2.74998161700885</v>
+      </c>
+      <c r="L53" t="n">
+        <v>40.68565000000001</v>
+      </c>
+      <c r="M53" t="n">
+        <v>90</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="n">
+        <v>24.5207625</v>
+      </c>
+      <c r="P53" t="n">
+        <v>17.9199</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0</v>
+      </c>
+      <c r="R53" t="n">
+        <v>2</v>
+      </c>
+      <c r="S53" t="n">
+        <v>90571</v>
+      </c>
+      <c r="T53" t="n">
+        <v>1</v>
+      </c>
+      <c r="U53" t="b">
+        <v>1</v>
+      </c>
+      <c r="V53" t="n">
+        <v>65</v>
+      </c>
+      <c r="W53" t="n">
+        <v>86</v>
+      </c>
+      <c r="X53" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB53" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE53" t="n">
+        <v>0.03412854453193988</v>
+      </c>
+      <c r="AF53" t="n">
+        <v>0.01456205218638635</v>
+      </c>
+      <c r="AG53" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C54" t="n">
+        <v>52</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-0.5909375</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.00109375</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.01584756904481133</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.02831660118739321</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.0002208278111527066</v>
+      </c>
+      <c r="I54" t="n">
+        <v>2</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>2.799999972796035</v>
+      </c>
+      <c r="L54" t="n">
+        <v>41.29310000000001</v>
+      </c>
+      <c r="M54" t="n">
+        <v>90</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>24.9949875</v>
+      </c>
+      <c r="P54" t="n">
+        <v>17.9050625</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0</v>
+      </c>
+      <c r="R54" t="n">
+        <v>2</v>
+      </c>
+      <c r="S54" t="n">
+        <v>90856</v>
+      </c>
+      <c r="T54" t="n">
+        <v>1</v>
+      </c>
+      <c r="U54" t="b">
+        <v>1</v>
+      </c>
+      <c r="V54" t="n">
+        <v>65</v>
+      </c>
+      <c r="W54" t="n">
+        <v>86</v>
+      </c>
+      <c r="X54" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB54" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC54" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE54" t="n">
+        <v>0.0308971157000648</v>
+      </c>
+      <c r="AF54" t="n">
+        <v>0.014839149746727</v>
+      </c>
+      <c r="AG54" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C55" t="n">
+        <v>53</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-0.5873437500000001</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.00109375</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.01193857096046969</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.02812218009329102</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.0002178064957862713</v>
+      </c>
+      <c r="I55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>2.849998220775606</v>
+      </c>
+      <c r="L55" t="n">
+        <v>41.9152</v>
+      </c>
+      <c r="M55" t="n">
+        <v>90</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>25.4707375</v>
+      </c>
+      <c r="P55" t="n">
+        <v>17.887325</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0</v>
+      </c>
+      <c r="R55" t="n">
+        <v>2</v>
+      </c>
+      <c r="S55" t="n">
+        <v>91603</v>
+      </c>
+      <c r="T55" t="n">
+        <v>1</v>
+      </c>
+      <c r="U55" t="b">
+        <v>1</v>
+      </c>
+      <c r="V55" t="n">
+        <v>65</v>
+      </c>
+      <c r="W55" t="n">
+        <v>86</v>
+      </c>
+      <c r="X55" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB55" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE55" t="n">
+        <v>0.03500953250804797</v>
+      </c>
+      <c r="AF55" t="n">
+        <v>0.01511517331133291</v>
+      </c>
+      <c r="AG55" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C56" t="n">
+        <v>54</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-0.589375</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.00109375</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.01480396412385132</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.0344646335140705</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.0002176266154960011</v>
+      </c>
+      <c r="I56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>2.899990503564362</v>
+      </c>
+      <c r="L56" t="n">
+        <v>42.552425</v>
+      </c>
+      <c r="M56" t="n">
+        <v>90</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>25.94815</v>
+      </c>
+      <c r="P56" t="n">
+        <v>17.8663125</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0</v>
+      </c>
+      <c r="R56" t="n">
+        <v>2</v>
+      </c>
+      <c r="S56" t="n">
+        <v>90013</v>
+      </c>
+      <c r="T56" t="n">
+        <v>1</v>
+      </c>
+      <c r="U56" t="b">
+        <v>1</v>
+      </c>
+      <c r="V56" t="n">
+        <v>65</v>
+      </c>
+      <c r="W56" t="n">
+        <v>86</v>
+      </c>
+      <c r="X56" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB56" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE56" t="n">
+        <v>0.04206193343255842</v>
+      </c>
+      <c r="AF56" t="n">
+        <v>0.01539010585544142</v>
+      </c>
+      <c r="AG56" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C57" t="n">
+        <v>55</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-0.5739062500000001</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-0.00078125</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.01442001404798264</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.02889807999156284</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.0002155427811010822</v>
+      </c>
+      <c r="I57" t="n">
+        <v>2</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>2.950003811929659</v>
+      </c>
+      <c r="L57" t="n">
+        <v>43.20542500000001</v>
+      </c>
+      <c r="M57" t="n">
+        <v>90</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>26.4276</v>
+      </c>
+      <c r="P57" t="n">
+        <v>17.8421</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0</v>
+      </c>
+      <c r="R57" t="n">
+        <v>2</v>
+      </c>
+      <c r="S57" t="n">
+        <v>90850</v>
+      </c>
+      <c r="T57" t="n">
+        <v>1</v>
+      </c>
+      <c r="U57" t="b">
+        <v>1</v>
+      </c>
+      <c r="V57" t="n">
+        <v>65</v>
+      </c>
+      <c r="W57" t="n">
+        <v>86</v>
+      </c>
+      <c r="X57" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB57" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC57" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE57" t="n">
+        <v>0.03375890282408303</v>
+      </c>
+      <c r="AF57" t="n">
+        <v>0.01566413067283448</v>
+      </c>
+      <c r="AG57" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C58" t="n">
+        <v>56</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-0.59140625</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.001171875</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.01655270049963092</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.03289045203824389</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.000214793851164561</v>
+      </c>
+      <c r="I58" t="n">
+        <v>2</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>3.000011703727758</v>
+      </c>
+      <c r="L58" t="n">
+        <v>43.874075</v>
+      </c>
+      <c r="M58" t="n">
+        <v>90</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>26.908775</v>
+      </c>
+      <c r="P58" t="n">
+        <v>17.8143375</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" t="n">
+        <v>2</v>
+      </c>
+      <c r="S58" t="n">
+        <v>90017</v>
+      </c>
+      <c r="T58" t="n">
+        <v>1</v>
+      </c>
+      <c r="U58" t="b">
+        <v>1</v>
+      </c>
+      <c r="V58" t="n">
+        <v>65</v>
+      </c>
+      <c r="W58" t="n">
+        <v>86</v>
+      </c>
+      <c r="X58" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB58" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC58" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE58" t="n">
+        <v>0.03695855875315981</v>
+      </c>
+      <c r="AF58" t="n">
+        <v>0.01593697164210393</v>
+      </c>
+      <c r="AG58" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C59" t="n">
+        <v>57</v>
+      </c>
+      <c r="D59" t="n">
+        <v>-0.5821875</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-0.0009375</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.01287534545602416</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.03129613448375958</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.0002138088692277964</v>
+      </c>
+      <c r="I59" t="n">
+        <v>2</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>3.049980189948096</v>
+      </c>
+      <c r="L59" t="n">
+        <v>44.55885000000001</v>
+      </c>
+      <c r="M59" t="n">
+        <v>90</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>27.3918125</v>
+      </c>
+      <c r="P59" t="n">
+        <v>17.7827875</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" t="n">
+        <v>2</v>
+      </c>
+      <c r="S59" t="n">
+        <v>89935</v>
+      </c>
+      <c r="T59" t="n">
+        <v>1</v>
+      </c>
+      <c r="U59" t="b">
+        <v>1</v>
+      </c>
+      <c r="V59" t="n">
+        <v>65</v>
+      </c>
+      <c r="W59" t="n">
+        <v>86</v>
+      </c>
+      <c r="X59" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB59" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC59" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE59" t="n">
+        <v>0.03718449410460145</v>
+      </c>
+      <c r="AF59" t="n">
+        <v>0.01620863056210001</v>
+      </c>
+      <c r="AG59" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C60" t="n">
+        <v>58</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-0.5903125</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.00109375</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.007634579083640014</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.03041914732840344</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.000215975708927441</v>
+      </c>
+      <c r="I60" t="n">
+        <v>2</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>3.099990225104579</v>
+      </c>
+      <c r="L60" t="n">
+        <v>45.26065000000001</v>
+      </c>
+      <c r="M60" t="n">
+        <v>90</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="n">
+        <v>27.87715</v>
+      </c>
+      <c r="P60" t="n">
+        <v>17.7472</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0</v>
+      </c>
+      <c r="R60" t="n">
+        <v>2</v>
+      </c>
+      <c r="S60" t="n">
+        <v>89311</v>
+      </c>
+      <c r="T60" t="n">
+        <v>1</v>
+      </c>
+      <c r="U60" t="b">
+        <v>1</v>
+      </c>
+      <c r="V60" t="n">
+        <v>65</v>
+      </c>
+      <c r="W60" t="n">
+        <v>86</v>
+      </c>
+      <c r="X60" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA60" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB60" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE60" t="n">
+        <v>0.03604421360411075</v>
+      </c>
+      <c r="AF60" t="n">
+        <v>0.0164792767436571</v>
+      </c>
+      <c r="AG60" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C61" t="n">
+        <v>59</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-0.592890625</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.00125</v>
+      </c>
+      <c r="F61" t="n">
+        <v>9.587927809848185e-05</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.0293291637580602</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.0002140201136161712</v>
+      </c>
+      <c r="I61" t="n">
+        <v>2</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>3.149987839202876</v>
+      </c>
+      <c r="L61" t="n">
+        <v>45.979075</v>
+      </c>
+      <c r="M61" t="n">
+        <v>90</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="n">
+        <v>28.364275</v>
+      </c>
+      <c r="P61" t="n">
+        <v>17.7073</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0</v>
+      </c>
+      <c r="R61" t="n">
+        <v>2</v>
+      </c>
+      <c r="S61" t="n">
+        <v>91946</v>
+      </c>
+      <c r="T61" t="n">
+        <v>1</v>
+      </c>
+      <c r="U61" t="b">
+        <v>1</v>
+      </c>
+      <c r="V61" t="n">
+        <v>65</v>
+      </c>
+      <c r="W61" t="n">
+        <v>86</v>
+      </c>
+      <c r="X61" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA61" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB61" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC61" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE61" t="n">
+        <v>0.03454661388723191</v>
+      </c>
+      <c r="AF61" t="n">
+        <v>0.01674853618580725</v>
+      </c>
+      <c r="AG61" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C62" t="n">
+        <v>60</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-0.581015625</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-0.001015625</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.00227869233058315</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.03041482626593658</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.0002155086945308865</v>
+      </c>
+      <c r="I62" t="n">
+        <v>2</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="n">
+        <v>3.200002349843249</v>
+      </c>
+      <c r="L62" t="n">
+        <v>46.71525</v>
+      </c>
+      <c r="M62" t="n">
+        <v>90</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="n">
+        <v>28.8537375</v>
+      </c>
+      <c r="P62" t="n">
+        <v>17.6628625</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>0</v>
+      </c>
+      <c r="R62" t="n">
+        <v>2</v>
+      </c>
+      <c r="S62" t="n">
+        <v>91032</v>
+      </c>
+      <c r="T62" t="n">
+        <v>1</v>
+      </c>
+      <c r="U62" t="b">
+        <v>1</v>
+      </c>
+      <c r="V62" t="n">
+        <v>65</v>
+      </c>
+      <c r="W62" t="n">
+        <v>86</v>
+      </c>
+      <c r="X62" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y62" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z62" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA62" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB62" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD62" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE62" t="n">
+        <v>0.03578891414706196</v>
+      </c>
+      <c r="AF62" t="n">
+        <v>0.01701664575733711</v>
+      </c>
+      <c r="AG62" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C63" t="n">
+        <v>61</v>
+      </c>
+      <c r="D63" t="n">
+        <v>-0.587734375</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-0.00125</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.0004615815303956605</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.03098783436360932</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.0002144908899104624</v>
+      </c>
+      <c r="I63" t="n">
+        <v>2</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="n">
+        <v>3.250006684077497</v>
+      </c>
+      <c r="L63" t="n">
+        <v>47.46905</v>
+      </c>
+      <c r="M63" t="n">
+        <v>90</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
+      <c r="O63" t="n">
+        <v>29.3450375</v>
+      </c>
+      <c r="P63" t="n">
+        <v>17.61325</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>0</v>
+      </c>
+      <c r="R63" t="n">
+        <v>2</v>
+      </c>
+      <c r="S63" t="n">
+        <v>91191</v>
+      </c>
+      <c r="T63" t="n">
+        <v>1</v>
+      </c>
+      <c r="U63" t="b">
+        <v>1</v>
+      </c>
+      <c r="V63" t="n">
+        <v>65</v>
+      </c>
+      <c r="W63" t="n">
+        <v>86</v>
+      </c>
+      <c r="X63" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y63" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z63" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA63" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB63" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD63" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE63" t="n">
+        <v>0.03680844633730744</v>
+      </c>
+      <c r="AF63" t="n">
+        <v>0.01728319189579479</v>
+      </c>
+      <c r="AG63" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C64" t="n">
+        <v>62</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-0.586171875</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.00109375</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.0005156467728352557</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.03591820975645529</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.0002179173603090783</v>
+      </c>
+      <c r="I64" t="n">
+        <v>2</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="n">
+        <v>3.299985501301866</v>
+      </c>
+      <c r="L64" t="n">
+        <v>48.241425</v>
+      </c>
+      <c r="M64" t="n">
+        <v>90</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="n">
+        <v>29.8386625</v>
+      </c>
+      <c r="P64" t="n">
+        <v>17.5583125</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0</v>
+      </c>
+      <c r="R64" t="n">
+        <v>2</v>
+      </c>
+      <c r="S64" t="n">
+        <v>90516</v>
+      </c>
+      <c r="T64" t="n">
+        <v>1</v>
+      </c>
+      <c r="U64" t="b">
+        <v>1</v>
+      </c>
+      <c r="V64" t="n">
+        <v>65</v>
+      </c>
+      <c r="W64" t="n">
+        <v>86</v>
+      </c>
+      <c r="X64" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y64" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z64" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA64" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB64" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC64" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD64" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE64" t="n">
+        <v>0.04265609142586059</v>
+      </c>
+      <c r="AF64" t="n">
+        <v>0.0175483878919428</v>
+      </c>
+      <c r="AG64" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C65" t="n">
+        <v>63</v>
+      </c>
+      <c r="D65" t="n">
+        <v>-0.58078125</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-0.001015625</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.01411349181604747</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.02674777695578947</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.0002144329717022947</v>
+      </c>
+      <c r="I65" t="n">
+        <v>2</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="n">
+        <v>3.349970737050941</v>
+      </c>
+      <c r="L65" t="n">
+        <v>49.0333</v>
+      </c>
+      <c r="M65" t="n">
+        <v>90</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="n">
+        <v>30.3348125</v>
+      </c>
+      <c r="P65" t="n">
+        <v>17.497525</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>0</v>
+      </c>
+      <c r="R65" t="n">
+        <v>2</v>
+      </c>
+      <c r="S65" t="n">
+        <v>89955</v>
+      </c>
+      <c r="T65" t="n">
+        <v>1</v>
+      </c>
+      <c r="U65" t="b">
+        <v>1</v>
+      </c>
+      <c r="V65" t="n">
+        <v>65</v>
+      </c>
+      <c r="W65" t="n">
+        <v>86</v>
+      </c>
+      <c r="X65" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y65" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z65" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA65" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB65" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC65" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD65" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE65" t="n">
+        <v>0.03625922052459175</v>
+      </c>
+      <c r="AF65" t="n">
+        <v>0.01781222953708385</v>
+      </c>
+      <c r="AG65" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C66" t="n">
+        <v>64</v>
+      </c>
+      <c r="D66" t="n">
+        <v>-0.581171875</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.0009375</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.002235285831962419</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.02889741408885714</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.0002162793660281577</v>
+      </c>
+      <c r="I66" t="n">
+        <v>2</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="n">
+        <v>3.400016015008965</v>
+      </c>
+      <c r="L66" t="n">
+        <v>49.84497500000001</v>
+      </c>
+      <c r="M66" t="n">
+        <v>90</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="n">
+        <v>30.8334125</v>
+      </c>
+      <c r="P66" t="n">
+        <v>17.430675</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>0</v>
+      </c>
+      <c r="R66" t="n">
+        <v>2</v>
+      </c>
+      <c r="S66" t="n">
+        <v>91298</v>
+      </c>
+      <c r="T66" t="n">
+        <v>1</v>
+      </c>
+      <c r="U66" t="b">
+        <v>1</v>
+      </c>
+      <c r="V66" t="n">
+        <v>65</v>
+      </c>
+      <c r="W66" t="n">
+        <v>86</v>
+      </c>
+      <c r="X66" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y66" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z66" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA66" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB66" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC66" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD66" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE66" t="n">
+        <v>0.03360491455188747</v>
+      </c>
+      <c r="AF66" t="n">
+        <v>0.01807460951695382</v>
+      </c>
+      <c r="AG66" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C67" t="n">
+        <v>65</v>
+      </c>
+      <c r="D67" t="n">
+        <v>-0.5896875</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.001015625</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.0112326643026261</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.03492046457265899</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.0002184491894306464</v>
+      </c>
+      <c r="I67" t="n">
+        <v>2</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="n">
+        <v>3.449989284016248</v>
+      </c>
+      <c r="L67" t="n">
+        <v>50.67685</v>
+      </c>
+      <c r="M67" t="n">
+        <v>90</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>31.334325</v>
+      </c>
+      <c r="P67" t="n">
+        <v>17.3572</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" t="n">
+        <v>2</v>
+      </c>
+      <c r="S67" t="n">
+        <v>91228</v>
+      </c>
+      <c r="T67" t="n">
+        <v>1</v>
+      </c>
+      <c r="U67" t="b">
+        <v>1</v>
+      </c>
+      <c r="V67" t="n">
+        <v>65</v>
+      </c>
+      <c r="W67" t="n">
+        <v>86</v>
+      </c>
+      <c r="X67" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y67" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z67" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA67" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB67" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC67" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD67" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE67" t="n">
+        <v>0.04035722042126912</v>
+      </c>
+      <c r="AF67" t="n">
+        <v>0.01833533978244691</v>
+      </c>
+      <c r="AG67" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C68" t="n">
+        <v>66</v>
+      </c>
+      <c r="D68" t="n">
+        <v>-0.5871875</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.00109375</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.01828371527050776</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.03136873050121229</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.0002174202466470541</v>
+      </c>
+      <c r="I68" t="n">
+        <v>2</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="n">
+        <v>3.500012087085825</v>
+      </c>
+      <c r="L68" t="n">
+        <v>51.52985</v>
+      </c>
+      <c r="M68" t="n">
+        <v>90</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="n">
+        <v>31.83775</v>
+      </c>
+      <c r="P68" t="n">
+        <v>17.276625</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>0</v>
+      </c>
+      <c r="R68" t="n">
+        <v>2</v>
+      </c>
+      <c r="S68" t="n">
+        <v>90256</v>
+      </c>
+      <c r="T68" t="n">
+        <v>1</v>
+      </c>
+      <c r="U68" t="b">
+        <v>1</v>
+      </c>
+      <c r="V68" t="n">
+        <v>65</v>
+      </c>
+      <c r="W68" t="n">
+        <v>86</v>
+      </c>
+      <c r="X68" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y68" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z68" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA68" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB68" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD68" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE68" t="n">
+        <v>0.0397505619848881</v>
+      </c>
+      <c r="AF68" t="n">
+        <v>0.0185944328516533</v>
+      </c>
+      <c r="AG68" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C69" t="n">
+        <v>67</v>
+      </c>
+      <c r="D69" t="n">
+        <v>-0.5921875</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0.001171875</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.02690605271513433</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.0355348740267374</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.0002197923596264416</v>
+      </c>
+      <c r="I69" t="n">
+        <v>2</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
+        <v>3.549978895841876</v>
+      </c>
+      <c r="L69" t="n">
+        <v>52.40485</v>
+      </c>
+      <c r="M69" t="n">
+        <v>90</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="n">
+        <v>32.3437</v>
+      </c>
+      <c r="P69" t="n">
+        <v>17.1882625</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0</v>
+      </c>
+      <c r="R69" t="n">
+        <v>2</v>
+      </c>
+      <c r="S69" t="n">
+        <v>90227</v>
+      </c>
+      <c r="T69" t="n">
+        <v>1</v>
+      </c>
+      <c r="U69" t="b">
+        <v>1</v>
+      </c>
+      <c r="V69" t="n">
+        <v>65</v>
+      </c>
+      <c r="W69" t="n">
+        <v>86</v>
+      </c>
+      <c r="X69" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y69" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z69" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA69" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB69" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD69" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE69" t="n">
+        <v>0.04353209260878627</v>
+      </c>
+      <c r="AF69" t="n">
+        <v>0.01885177205728208</v>
+      </c>
+      <c r="AG69" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C70" t="n">
+        <v>68</v>
+      </c>
+      <c r="D70" t="n">
+        <v>-0.58421875</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.001015625</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.02286671857393395</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.0312295099169916</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.0002229243296185334</v>
+      </c>
+      <c r="I70" t="n">
+        <v>2</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="n">
+        <v>3.599997095962363</v>
+      </c>
+      <c r="L70" t="n">
+        <v>53.303125</v>
+      </c>
+      <c r="M70" t="n">
+        <v>90</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="n">
+        <v>32.8526</v>
+      </c>
+      <c r="P70" t="n">
+        <v>17.0917</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0</v>
+      </c>
+      <c r="R70" t="n">
+        <v>2</v>
+      </c>
+      <c r="S70" t="n">
+        <v>90158</v>
+      </c>
+      <c r="T70" t="n">
+        <v>1</v>
+      </c>
+      <c r="U70" t="b">
+        <v>1</v>
+      </c>
+      <c r="V70" t="n">
+        <v>65</v>
+      </c>
+      <c r="W70" t="n">
+        <v>86</v>
+      </c>
+      <c r="X70" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y70" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z70" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA70" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB70" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC70" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD70" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE70" t="n">
+        <v>0.03889831904573888</v>
+      </c>
+      <c r="AF70" t="n">
+        <v>0.01910750496657658</v>
+      </c>
+      <c r="AG70" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C71" t="n">
+        <v>69</v>
+      </c>
+      <c r="D71" t="n">
+        <v>-0.586953125</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.00125</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.02663781661744244</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.02925802482472363</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.0002247108483670509</v>
+      </c>
+      <c r="I71" t="n">
+        <v>2</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="n">
+        <v>3.649989781390765</v>
+      </c>
+      <c r="L71" t="n">
+        <v>54.225375</v>
+      </c>
+      <c r="M71" t="n">
+        <v>90</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="n">
+        <v>33.3642875</v>
+      </c>
+      <c r="P71" t="n">
+        <v>16.9862625</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>0</v>
+      </c>
+      <c r="R71" t="n">
+        <v>2</v>
+      </c>
+      <c r="S71" t="n">
+        <v>90525</v>
+      </c>
+      <c r="T71" t="n">
+        <v>1</v>
+      </c>
+      <c r="U71" t="b">
+        <v>1</v>
+      </c>
+      <c r="V71" t="n">
+        <v>65</v>
+      </c>
+      <c r="W71" t="n">
+        <v>86</v>
+      </c>
+      <c r="X71" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z71" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA71" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB71" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC71" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD71" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE71" t="n">
+        <v>0.03667676683969844</v>
+      </c>
+      <c r="AF71" t="n">
+        <v>0.01936143228450777</v>
+      </c>
+      <c r="AG71" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C72" t="n">
+        <v>70</v>
+      </c>
+      <c r="D72" t="n">
+        <v>-0.5878125</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-0.000703125</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.03275918584089961</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.03080661044210855</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.0002315802811312316</v>
+      </c>
+      <c r="I72" t="n">
+        <v>2</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="n">
+        <v>3.699987832535496</v>
+      </c>
+      <c r="L72" t="n">
+        <v>55.17227500000001</v>
+      </c>
+      <c r="M72" t="n">
+        <v>90</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="n">
+        <v>33.8786375</v>
+      </c>
+      <c r="P72" t="n">
+        <v>16.871225</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>0</v>
+      </c>
+      <c r="R72" t="n">
+        <v>2</v>
+      </c>
+      <c r="S72" t="n">
+        <v>89943</v>
+      </c>
+      <c r="T72" t="n">
+        <v>1</v>
+      </c>
+      <c r="U72" t="b">
+        <v>1</v>
+      </c>
+      <c r="V72" t="n">
+        <v>65</v>
+      </c>
+      <c r="W72" t="n">
+        <v>86</v>
+      </c>
+      <c r="X72" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y72" t="n">
+        <v>246</v>
+      </c>
+      <c r="Z72" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA72" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB72" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC72" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD72" t="inlineStr">
+        <is>
+          <t>traditional</t>
+        </is>
+      </c>
+      <c r="AE72" t="n">
+        <v>0.03843676598678051</v>
+      </c>
+      <c r="AF72" t="n">
+        <v>0.01961337738772106</v>
+      </c>
+      <c r="AG72" t="n">
+        <v>-20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new tab in viewer to obtain charge of a specified peak in CV profile
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_ctr.xlsx
+++ b/dump_files/temp_data_ctr.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG19"/>
+  <dimension ref="A1:AG39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,13 +613,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05467071789568272</v>
+        <v>0.09721576304624097</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00615024699254615</v>
+        <v>0.01162994378862035</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0002729130270251847</v>
+        <v>0.0002542914692872765</v>
       </c>
       <c r="I2" t="n">
         <v>2</v>
@@ -661,16 +661,16 @@
         <v>1</v>
       </c>
       <c r="V2" t="n">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="W2" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
         <v>120</v>
       </c>
       <c r="Y2" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z2" t="n">
         <v>2</v>
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="AE2" t="n">
-        <v>0.03922705165821064</v>
+        <v>0.1135486862779087</v>
       </c>
       <c r="AF2" t="n">
         <v>0.0001589856854948248</v>
@@ -718,13 +718,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2830958436253628</v>
+        <v>0.3604410818283874</v>
       </c>
       <c r="G3" t="n">
-        <v>0.006486442766384275</v>
+        <v>0.0122455345470943</v>
       </c>
       <c r="H3" t="n">
-        <v>0.000282316006173504</v>
+        <v>0.0002772119912235288</v>
       </c>
       <c r="I3" t="n">
         <v>2</v>
@@ -766,16 +766,16 @@
         <v>1</v>
       </c>
       <c r="V3" t="n">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="W3" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
         <v>120</v>
       </c>
       <c r="Y3" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z3" t="n">
         <v>2</v>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="AE3" t="n">
-        <v>0.04637760697642813</v>
+        <v>0.1680814628053406</v>
       </c>
       <c r="AF3" t="n">
         <v>0.0001335700357694114</v>
@@ -823,13 +823,13 @@
         <v>-0.00125</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3051682889241764</v>
+        <v>0.4292451383095024</v>
       </c>
       <c r="G4" t="n">
-        <v>0.006505022765037007</v>
+        <v>0.01245976932937304</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0002846520430304953</v>
+        <v>0.0002765234039743844</v>
       </c>
       <c r="I4" t="n">
         <v>2</v>
@@ -871,19 +871,19 @@
         <v>1</v>
       </c>
       <c r="V4" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W4" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
         <v>120</v>
       </c>
       <c r="Y4" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z4" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA4" t="n">
         <v>30</v>
@@ -894,15 +894,15 @@
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE4" t="n">
-        <v>0.04806539658228844</v>
+        <v>0.07310918426250616</v>
       </c>
       <c r="AF4" t="n">
         <v>0.0004261338930113039</v>
@@ -928,13 +928,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2193532781346333</v>
+        <v>0.3867784769656659</v>
       </c>
       <c r="G5" t="n">
-        <v>0.006423951537349833</v>
+        <v>0.01255939959506199</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0002824272370779774</v>
+        <v>0.0002800113208656786</v>
       </c>
       <c r="I5" t="n">
         <v>2</v>
@@ -976,19 +976,19 @@
         <v>1</v>
       </c>
       <c r="V5" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W5" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
         <v>120</v>
       </c>
       <c r="Y5" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z5" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA5" t="n">
         <v>30</v>
@@ -999,15 +999,15 @@
         </is>
       </c>
       <c r="AC5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE5" t="n">
-        <v>0.0492409403761126</v>
+        <v>0.07987328045400129</v>
       </c>
       <c r="AF5" t="n">
         <v>0.000718676592156832</v>
@@ -1033,13 +1033,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1364860405632867</v>
+        <v>0.2482534556277327</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00633441575073987</v>
+        <v>0.01247317206349413</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000280296790625013</v>
+        <v>0.0002796405016381445</v>
       </c>
       <c r="I6" t="n">
         <v>2</v>
@@ -1081,19 +1081,19 @@
         <v>1</v>
       </c>
       <c r="V6" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W6" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
         <v>120</v>
       </c>
       <c r="Y6" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z6" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA6" t="n">
         <v>30</v>
@@ -1104,15 +1104,15 @@
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE6" t="n">
-        <v>0.04296558890359705</v>
+        <v>0.08261635290790187</v>
       </c>
       <c r="AF6" t="n">
         <v>0.001011189028630286</v>
@@ -1138,13 +1138,13 @@
         <v>-0.001328125</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1155480270476729</v>
+        <v>0.1433588034992892</v>
       </c>
       <c r="G7" t="n">
-        <v>0.006303366002857194</v>
+        <v>0.01242578130693887</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0002776336997970481</v>
+        <v>0.0002777180935504116</v>
       </c>
       <c r="I7" t="n">
         <v>2</v>
@@ -1186,19 +1186,19 @@
         <v>1</v>
       </c>
       <c r="V7" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W7" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
         <v>120</v>
       </c>
       <c r="Y7" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z7" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA7" t="n">
         <v>30</v>
@@ -1209,15 +1209,15 @@
         </is>
       </c>
       <c r="AC7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE7" t="n">
-        <v>0.04065986440327164</v>
+        <v>0.0729184167211837</v>
       </c>
       <c r="AF7" t="n">
         <v>0.001303701231108943</v>
@@ -1243,13 +1243,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F8" t="n">
-        <v>0.09144245598302218</v>
+        <v>0.1101531280681252</v>
       </c>
       <c r="G8" t="n">
-        <v>0.006245084442922998</v>
+        <v>0.01233789861123646</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0002719606394387458</v>
+        <v>0.0002741681960461386</v>
       </c>
       <c r="I8" t="n">
         <v>2</v>
@@ -1291,19 +1291,19 @@
         <v>1</v>
       </c>
       <c r="V8" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W8" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
         <v>120</v>
       </c>
       <c r="Y8" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z8" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA8" t="n">
         <v>30</v>
@@ -1314,15 +1314,15 @@
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE8" t="n">
-        <v>0.04293397270958584</v>
+        <v>0.08289299188891797</v>
       </c>
       <c r="AF8" t="n">
         <v>0.001596208987665999</v>
@@ -1348,13 +1348,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F9" t="n">
-        <v>0.07443918990891593</v>
+        <v>0.04721323578668998</v>
       </c>
       <c r="G9" t="n">
-        <v>0.006237097652493641</v>
+        <v>0.01229065327816423</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0002714473208126259</v>
+        <v>0.0002727098564201884</v>
       </c>
       <c r="I9" t="n">
         <v>2</v>
@@ -1396,19 +1396,19 @@
         <v>1</v>
       </c>
       <c r="V9" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W9" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
         <v>120</v>
       </c>
       <c r="Y9" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z9" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA9" t="n">
         <v>30</v>
@@ -1419,15 +1419,15 @@
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE9" t="n">
-        <v>0.04245027356696485</v>
+        <v>0.07165492555935239</v>
       </c>
       <c r="AF9" t="n">
         <v>0.001888642857126413</v>
@@ -1453,13 +1453,13 @@
         <v>-0.001015625</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05581059292277708</v>
+        <v>-0.01208541827247678</v>
       </c>
       <c r="G10" t="n">
-        <v>0.006182262519637372</v>
+        <v>0.01217182094252085</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0002713103743997844</v>
+        <v>0.0002691485194569915</v>
       </c>
       <c r="I10" t="n">
         <v>2</v>
@@ -1501,19 +1501,19 @@
         <v>1</v>
       </c>
       <c r="V10" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W10" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
         <v>120</v>
       </c>
       <c r="Y10" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z10" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA10" t="n">
         <v>30</v>
@@ -1524,15 +1524,15 @@
         </is>
       </c>
       <c r="AC10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE10" t="n">
-        <v>0.04276793723647929</v>
+        <v>0.08001684561983895</v>
       </c>
       <c r="AF10" t="n">
         <v>0.002181063517051033</v>
@@ -1558,13 +1558,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F11" t="n">
-        <v>0.05733603224821522</v>
+        <v>-0.02112701548918393</v>
       </c>
       <c r="G11" t="n">
-        <v>0.006183473216571376</v>
+        <v>0.01219559275913333</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0002694322468841027</v>
+        <v>0.0002681817343003193</v>
       </c>
       <c r="I11" t="n">
         <v>2</v>
@@ -1606,19 +1606,19 @@
         <v>1</v>
       </c>
       <c r="V11" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W11" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X11" t="n">
         <v>120</v>
       </c>
       <c r="Y11" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z11" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA11" t="n">
         <v>30</v>
@@ -1629,15 +1629,15 @@
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE11" t="n">
-        <v>0.04403241263138627</v>
+        <v>0.08328248406425358</v>
       </c>
       <c r="AF11" t="n">
         <v>0.002473415448778893</v>
@@ -1663,13 +1663,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F12" t="n">
-        <v>0.05086398129847272</v>
+        <v>-0.09940510848095546</v>
       </c>
       <c r="G12" t="n">
-        <v>0.00618435868592918</v>
+        <v>0.01219194482485311</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0002690677289887083</v>
+        <v>0.0002688227140323746</v>
       </c>
       <c r="I12" t="n">
         <v>2</v>
@@ -1711,19 +1711,19 @@
         <v>1</v>
       </c>
       <c r="V12" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W12" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X12" t="n">
         <v>120</v>
       </c>
       <c r="Y12" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z12" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA12" t="n">
         <v>30</v>
@@ -1734,15 +1734,15 @@
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE12" t="n">
-        <v>0.04399045551597572</v>
+        <v>0.07327882583760284</v>
       </c>
       <c r="AF12" t="n">
         <v>0.002765730954260923</v>
@@ -1768,13 +1768,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F13" t="n">
-        <v>0.04693522162169408</v>
+        <v>-0.07346311103086524</v>
       </c>
       <c r="G13" t="n">
-        <v>0.006165894326287903</v>
+        <v>0.01214924275918893</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0002672250270608704</v>
+        <v>0.0002658331237455556</v>
       </c>
       <c r="I13" t="n">
         <v>2</v>
@@ -1816,19 +1816,19 @@
         <v>1</v>
       </c>
       <c r="V13" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W13" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X13" t="n">
         <v>120</v>
       </c>
       <c r="Y13" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z13" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA13" t="n">
         <v>30</v>
@@ -1839,15 +1839,15 @@
         </is>
       </c>
       <c r="AC13" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE13" t="n">
-        <v>0.04177138337761545</v>
+        <v>0.07538156418293805</v>
       </c>
       <c r="AF13" t="n">
         <v>0.003058037269159208</v>
@@ -1873,13 +1873,13 @@
         <v>-0.001171875</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04236287266846538</v>
+        <v>-0.01875377261999316</v>
       </c>
       <c r="G14" t="n">
-        <v>0.006107155775322979</v>
+        <v>0.01201702572002968</v>
       </c>
       <c r="H14" t="n">
-        <v>0.000264178340509192</v>
+        <v>0.0002620080907157143</v>
       </c>
       <c r="I14" t="n">
         <v>2</v>
@@ -1921,19 +1921,19 @@
         <v>1</v>
       </c>
       <c r="V14" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W14" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X14" t="n">
         <v>120</v>
       </c>
       <c r="Y14" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z14" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA14" t="n">
         <v>30</v>
@@ -1944,15 +1944,15 @@
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE14" t="n">
-        <v>0.04214829176314138</v>
+        <v>0.07193499711820414</v>
       </c>
       <c r="AF14" t="n">
         <v>0.003350170867517325</v>
@@ -1978,13 +1978,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F15" t="n">
-        <v>0.04720240667461247</v>
+        <v>-0.09158662570116134</v>
       </c>
       <c r="G15" t="n">
-        <v>0.006099745060798177</v>
+        <v>0.0119987742954958</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0002624991034734545</v>
+        <v>0.0002613494819829722</v>
       </c>
       <c r="I15" t="n">
         <v>2</v>
@@ -2026,19 +2026,19 @@
         <v>1</v>
       </c>
       <c r="V15" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W15" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X15" t="n">
         <v>120</v>
       </c>
       <c r="Y15" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z15" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA15" t="n">
         <v>30</v>
@@ -2049,15 +2049,15 @@
         </is>
       </c>
       <c r="AC15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE15" t="n">
-        <v>0.04279554081059342</v>
+        <v>0.07315601240962116</v>
       </c>
       <c r="AF15" t="n">
         <v>0.003642322582859247</v>
@@ -2083,13 +2083,13 @@
         <v>-0.00109375</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0495200207359109</v>
+        <v>0.0268965623039755</v>
       </c>
       <c r="G16" t="n">
-        <v>0.006137244077133973</v>
+        <v>0.01207802757291996</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0002647845126864978</v>
+        <v>0.0002629780968157555</v>
       </c>
       <c r="I16" t="n">
         <v>2</v>
@@ -2131,19 +2131,19 @@
         <v>1</v>
       </c>
       <c r="V16" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W16" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X16" t="n">
         <v>120</v>
       </c>
       <c r="Y16" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z16" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA16" t="n">
         <v>30</v>
@@ -2154,15 +2154,15 @@
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD16" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE16" t="n">
-        <v>0.04341063817547596</v>
+        <v>0.08319230685289075</v>
       </c>
       <c r="AF16" t="n">
         <v>0.003934380251146528</v>
@@ -2188,13 +2188,13 @@
         <v>-0.0009375</v>
       </c>
       <c r="F17" t="n">
-        <v>0.04264741704083271</v>
+        <v>-0.09374473329677441</v>
       </c>
       <c r="G17" t="n">
-        <v>0.006102657297026548</v>
+        <v>0.01199294242278427</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0002615676991925946</v>
+        <v>0.0002597491035482739</v>
       </c>
       <c r="I17" t="n">
         <v>2</v>
@@ -2236,19 +2236,19 @@
         <v>1</v>
       </c>
       <c r="V17" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W17" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X17" t="n">
         <v>120</v>
       </c>
       <c r="Y17" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z17" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA17" t="n">
         <v>30</v>
@@ -2259,15 +2259,15 @@
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE17" t="n">
-        <v>0.04194985434696671</v>
+        <v>0.0736033256963585</v>
       </c>
       <c r="AF17" t="n">
         <v>0.004226326624840558</v>
@@ -2293,13 +2293,13 @@
         <v>-0.000859375</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0463417272101832</v>
+        <v>-0.0410041276867326</v>
       </c>
       <c r="G18" t="n">
-        <v>0.006164169457192132</v>
+        <v>0.01212338210220817</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0002640978478880761</v>
+        <v>0.0002629405572112747</v>
       </c>
       <c r="I18" t="n">
         <v>2</v>
@@ -2341,19 +2341,19 @@
         <v>1</v>
       </c>
       <c r="V18" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W18" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X18" t="n">
         <v>120</v>
       </c>
       <c r="Y18" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z18" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA18" t="n">
         <v>30</v>
@@ -2364,15 +2364,15 @@
         </is>
       </c>
       <c r="AC18" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE18" t="n">
-        <v>0.03741324317644645</v>
+        <v>0.07008889439947118</v>
       </c>
       <c r="AF18" t="n">
         <v>0.004518227805618716</v>
@@ -2398,13 +2398,13 @@
         <v>-0.00078125</v>
       </c>
       <c r="F19" t="n">
-        <v>0.03633506395678045</v>
+        <v>-0.08317999684882926</v>
       </c>
       <c r="G19" t="n">
-        <v>0.006204693915506917</v>
+        <v>0.01212218214869982</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0002771280853801693</v>
+        <v>0.0002635149620036074</v>
       </c>
       <c r="I19" t="n">
         <v>2</v>
@@ -2446,19 +2446,19 @@
         <v>1</v>
       </c>
       <c r="V19" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="W19" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="X19" t="n">
         <v>120</v>
       </c>
       <c r="Y19" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Z19" t="n">
-        <v>2</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="AA19" t="n">
         <v>30</v>
@@ -2469,20 +2469,2114 @@
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
-          <t>traditional</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="AE19" t="n">
-        <v>0.04882157856487492</v>
+        <v>0.08213484782894796</v>
       </c>
       <c r="AF19" t="n">
         <v>0.004809998234665402</v>
       </c>
       <c r="AG19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.591328125</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.001015625</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-0.07313909398545676</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0120927470184411</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.0002633318380593795</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.100000980117384</v>
+      </c>
+      <c r="L20" t="n">
+        <v>27.87910000000001</v>
+      </c>
+      <c r="M20" t="n">
+        <v>90</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>9.551587499999998</v>
+      </c>
+      <c r="P20" t="n">
+        <v>17.6960875</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>2</v>
+      </c>
+      <c r="S20" t="n">
+        <v>90656</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" t="b">
+        <v>1</v>
+      </c>
+      <c r="V20" t="n">
+        <v>29</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC20" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.07690185977316236</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0.005101681710295304</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.588515625</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-0.001171875</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-0.06444500903872252</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.01220351901041148</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0002657811560976695</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1.149996607987808</v>
+      </c>
+      <c r="L21" t="n">
+        <v>28.078075</v>
+      </c>
+      <c r="M21" t="n">
+        <v>90</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>9.992299999999998</v>
+      </c>
+      <c r="P21" t="n">
+        <v>17.708175</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>2</v>
+      </c>
+      <c r="S21" t="n">
+        <v>89854</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1</v>
+      </c>
+      <c r="U21" t="b">
+        <v>1</v>
+      </c>
+      <c r="V21" t="n">
+        <v>29</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC21" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.07673167673936901</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0.005393211541889114</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0.589765625</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.000625</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-0.1196532815589749</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.01214234805781315</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.0002662524286080868</v>
+      </c>
+      <c r="I22" t="n">
+        <v>2</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1.199988025867</v>
+      </c>
+      <c r="L22" t="n">
+        <v>28.28830000000001</v>
+      </c>
+      <c r="M22" t="n">
+        <v>90</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>10.433475</v>
+      </c>
+      <c r="P22" t="n">
+        <v>17.720525</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>2</v>
+      </c>
+      <c r="S22" t="n">
+        <v>90930</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1</v>
+      </c>
+      <c r="U22" t="b">
+        <v>1</v>
+      </c>
+      <c r="V22" t="n">
+        <v>29</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0</v>
+      </c>
+      <c r="X22" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC22" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE22" t="n">
+        <v>0.07084719773594624</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0.00568460021300261</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-0.582734375</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.00125</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-0.07998067493490235</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.01222512167336923</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.0002676845384586056</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1.249993639714321</v>
+      </c>
+      <c r="L23" t="n">
+        <v>28.50985</v>
+      </c>
+      <c r="M23" t="n">
+        <v>90</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>10.8751875</v>
+      </c>
+      <c r="P23" t="n">
+        <v>17.7330875</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>2</v>
+      </c>
+      <c r="S23" t="n">
+        <v>90341</v>
+      </c>
+      <c r="T23" t="n">
+        <v>1</v>
+      </c>
+      <c r="U23" t="b">
+        <v>1</v>
+      </c>
+      <c r="V23" t="n">
+        <v>29</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC23" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE23" t="n">
+        <v>0.07701719775504737</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0.005975866688449988</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.591875</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.001171875</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.09968058177228531</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.01227593944488667</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.000269854835467453</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1.299994417784478</v>
+      </c>
+      <c r="L24" t="n">
+        <v>28.7427</v>
+      </c>
+      <c r="M24" t="n">
+        <v>90</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>11.3174625</v>
+      </c>
+      <c r="P24" t="n">
+        <v>17.745825</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>2</v>
+      </c>
+      <c r="S24" t="n">
+        <v>90097</v>
+      </c>
+      <c r="T24" t="n">
+        <v>1</v>
+      </c>
+      <c r="U24" t="b">
+        <v>1</v>
+      </c>
+      <c r="V24" t="n">
+        <v>29</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC24" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE24" t="n">
+        <v>0.07443010337993071</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>0.00626699700686289</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-0.581015625</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-0.001328125</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-0.02968245353030034</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.01230393959507058</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0002715667387409952</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1.350000694082829</v>
+      </c>
+      <c r="L25" t="n">
+        <v>28.98695000000001</v>
+      </c>
+      <c r="M25" t="n">
+        <v>90</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>11.760325</v>
+      </c>
+      <c r="P25" t="n">
+        <v>17.75875</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>2</v>
+      </c>
+      <c r="S25" t="n">
+        <v>90493</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" t="b">
+        <v>1</v>
+      </c>
+      <c r="V25" t="n">
+        <v>29</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC25" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE25" t="n">
+        <v>0.08239212671015037</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>0.006557980366834047</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C26" t="n">
+        <v>24</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.58921875</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-0.001171875</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-0.1175461511694303</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.01228398291454161</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0002718803682332731</v>
+      </c>
+      <c r="I26" t="n">
+        <v>2</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1.400006572022451</v>
+      </c>
+      <c r="L26" t="n">
+        <v>29.242575</v>
+      </c>
+      <c r="M26" t="n">
+        <v>90</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>12.2037875</v>
+      </c>
+      <c r="P26" t="n">
+        <v>17.771725</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>2</v>
+      </c>
+      <c r="S26" t="n">
+        <v>90812</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1</v>
+      </c>
+      <c r="U26" t="b">
+        <v>1</v>
+      </c>
+      <c r="V26" t="n">
+        <v>29</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC26" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE26" t="n">
+        <v>0.08600428909539994</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>0.006848785725417059</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.58046875</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-0.001171875</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-0.09645049918755588</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.01236054492682397</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.0002741377001981253</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1.450004933582452</v>
+      </c>
+      <c r="L27" t="n">
+        <v>29.509575</v>
+      </c>
+      <c r="M27" t="n">
+        <v>90</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>12.6477875</v>
+      </c>
+      <c r="P27" t="n">
+        <v>17.7847625</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>2</v>
+      </c>
+      <c r="S27" t="n">
+        <v>90459</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1</v>
+      </c>
+      <c r="U27" t="b">
+        <v>1</v>
+      </c>
+      <c r="V27" t="n">
+        <v>29</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC27" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE27" t="n">
+        <v>0.07208338046461979</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0.007139343835434949</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.5873437500000001</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.00109375</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-0.05236184726711769</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.01236532268507459</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.0002754601399250201</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1.500000328136944</v>
+      </c>
+      <c r="L28" t="n">
+        <v>29.788</v>
+      </c>
+      <c r="M28" t="n">
+        <v>90</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>13.092425</v>
+      </c>
+      <c r="P28" t="n">
+        <v>17.79765</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>2</v>
+      </c>
+      <c r="S28" t="n">
+        <v>91017</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1</v>
+      </c>
+      <c r="U28" t="b">
+        <v>1</v>
+      </c>
+      <c r="V28" t="n">
+        <v>29</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC28" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE28" t="n">
+        <v>0.07071595618677998</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>0.007429672231614669</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C29" t="n">
+        <v>27</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-0.587734375</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-0.001015625</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.04884662776080657</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.01247246810724562</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.0002789036971766347</v>
+      </c>
+      <c r="I29" t="n">
+        <v>2</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1.550003706075667</v>
+      </c>
+      <c r="L29" t="n">
+        <v>30.078</v>
+      </c>
+      <c r="M29" t="n">
+        <v>90</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>13.5378625</v>
+      </c>
+      <c r="P29" t="n">
+        <v>17.810575</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>2</v>
+      </c>
+      <c r="S29" t="n">
+        <v>90790</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1</v>
+      </c>
+      <c r="U29" t="b">
+        <v>1</v>
+      </c>
+      <c r="V29" t="n">
+        <v>29</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC29" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE29" t="n">
+        <v>0.08173158649241107</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>0.007719861208897987</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C30" t="n">
+        <v>28</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-0.586953125</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-0.001015625</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-0.05265238702576254</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.0125066232744487</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.0002798235583019961</v>
+      </c>
+      <c r="I30" t="n">
+        <v>2</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1.600001924696995</v>
+      </c>
+      <c r="L30" t="n">
+        <v>30.37950000000001</v>
+      </c>
+      <c r="M30" t="n">
+        <v>90</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>13.9839125</v>
+      </c>
+      <c r="P30" t="n">
+        <v>17.8234125</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>2</v>
+      </c>
+      <c r="S30" t="n">
+        <v>90946</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1</v>
+      </c>
+      <c r="U30" t="b">
+        <v>1</v>
+      </c>
+      <c r="V30" t="n">
+        <v>29</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC30" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE30" t="n">
+        <v>0.08498850212232345</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>0.008009747283939044</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C31" t="n">
+        <v>29</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-0.59375</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-0.00078125</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.01451318158059961</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.01261108391060358</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.0002825859351752868</v>
+      </c>
+      <c r="I31" t="n">
+        <v>2</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1.650008818508131</v>
+      </c>
+      <c r="L31" t="n">
+        <v>30.6927</v>
+      </c>
+      <c r="M31" t="n">
+        <v>90</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>14.4308125</v>
+      </c>
+      <c r="P31" t="n">
+        <v>17.8362</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>2</v>
+      </c>
+      <c r="S31" t="n">
+        <v>90737</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1</v>
+      </c>
+      <c r="U31" t="b">
+        <v>1</v>
+      </c>
+      <c r="V31" t="n">
+        <v>29</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC31" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE31" t="n">
+        <v>0.08816573620666938</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>0.008299456036458841</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C32" t="n">
+        <v>30</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-0.5875781250000001</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-0.00125</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.1129759210342778</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.01280643109942381</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.0002896562592747939</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1.700002817181012</v>
+      </c>
+      <c r="L32" t="n">
+        <v>31.017425</v>
+      </c>
+      <c r="M32" t="n">
+        <v>90</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>14.8783625</v>
+      </c>
+      <c r="P32" t="n">
+        <v>17.848575</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>2</v>
+      </c>
+      <c r="S32" t="n">
+        <v>90598</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1</v>
+      </c>
+      <c r="U32" t="b">
+        <v>1</v>
+      </c>
+      <c r="V32" t="n">
+        <v>29</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC32" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE32" t="n">
+        <v>0.08265869300122752</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>0.00858879184594641</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C33" t="n">
+        <v>31</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-0.579921875</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-0.001171875</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.1471747613270381</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.01312806800828217</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.00029965071796862</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1.749996192199123</v>
+      </c>
+      <c r="L33" t="n">
+        <v>31.3539</v>
+      </c>
+      <c r="M33" t="n">
+        <v>90</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>15.3267875</v>
+      </c>
+      <c r="P33" t="n">
+        <v>17.8606875</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>2</v>
+      </c>
+      <c r="S33" t="n">
+        <v>90185</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1</v>
+      </c>
+      <c r="U33" t="b">
+        <v>1</v>
+      </c>
+      <c r="V33" t="n">
+        <v>29</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC33" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE33" t="n">
+        <v>0.08758760094039675</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0.008877879897123431</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C34" t="n">
+        <v>32</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-0.593671875</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-0.000703125</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.3558010329839981</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.01355287717185936</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.0003133899062735873</v>
+      </c>
+      <c r="I34" t="n">
+        <v>2</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1.799993564458712</v>
+      </c>
+      <c r="L34" t="n">
+        <v>31.70225000000001</v>
+      </c>
+      <c r="M34" t="n">
+        <v>90</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>15.7761125</v>
+      </c>
+      <c r="P34" t="n">
+        <v>17.872625</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>2</v>
+      </c>
+      <c r="S34" t="n">
+        <v>90974</v>
+      </c>
+      <c r="T34" t="n">
+        <v>1</v>
+      </c>
+      <c r="U34" t="b">
+        <v>1</v>
+      </c>
+      <c r="V34" t="n">
+        <v>29</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC34" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE34" t="n">
+        <v>0.09309470967324862</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0.009166711083625869</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C35" t="n">
+        <v>33</v>
+      </c>
+      <c r="D35" t="n">
+        <v>-0.58078125</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-0.00078125</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.7453436530178428</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.01499626186107222</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.0003575242183053706</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1.849983299104895</v>
+      </c>
+      <c r="L35" t="n">
+        <v>32.06235000000001</v>
+      </c>
+      <c r="M35" t="n">
+        <v>90</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>16.226225</v>
+      </c>
+      <c r="P35" t="n">
+        <v>17.8840875</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>2</v>
+      </c>
+      <c r="S35" t="n">
+        <v>91173</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="b">
+        <v>1</v>
+      </c>
+      <c r="V35" t="n">
+        <v>29</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC35" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE35" t="n">
+        <v>0.104444621842182</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0.00945514894295787</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C36" t="n">
+        <v>34</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-0.582109375</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.00125</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.824388978543791</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.02205070673315188</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.0006019511599511599</v>
+      </c>
+      <c r="I36" t="n">
+        <v>2</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1.899990609303646</v>
+      </c>
+      <c r="L36" t="n">
+        <v>32.4344</v>
+      </c>
+      <c r="M36" t="n">
+        <v>90</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>16.6773</v>
+      </c>
+      <c r="P36" t="n">
+        <v>17.89505</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>2</v>
+      </c>
+      <c r="S36" t="n">
+        <v>91000</v>
+      </c>
+      <c r="T36" t="n">
+        <v>1</v>
+      </c>
+      <c r="U36" t="b">
+        <v>1</v>
+      </c>
+      <c r="V36" t="n">
+        <v>29</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0</v>
+      </c>
+      <c r="X36" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC36" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD36" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE36" t="n">
+        <v>0.3682529781479076</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>0.009743266832289132</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C37" t="n">
+        <v>35</v>
+      </c>
+      <c r="D37" t="n">
+        <v>-0.58921875</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-0.000859375</v>
+      </c>
+      <c r="F37" t="n">
+        <v>5.928356976345359</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.1716905395692279</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.001302303469676041</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1.949989017990179</v>
+      </c>
+      <c r="L37" t="n">
+        <v>32.8184</v>
+      </c>
+      <c r="M37" t="n">
+        <v>90</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>17.129275</v>
+      </c>
+      <c r="P37" t="n">
+        <v>17.9054125</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>2</v>
+      </c>
+      <c r="S37" t="n">
+        <v>91071</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0.02796465868565877</v>
+      </c>
+      <c r="U37" t="b">
+        <v>1</v>
+      </c>
+      <c r="V37" t="n">
+        <v>29</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0</v>
+      </c>
+      <c r="X37" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC37" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD37" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE37" t="n">
+        <v>1.274734048233385</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>0.0100309779327597</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C38" t="n">
+        <v>36</v>
+      </c>
+      <c r="D38" t="n">
+        <v>-0.581171875</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.0009375</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>2</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1.999990868120535</v>
+      </c>
+      <c r="L38" t="n">
+        <v>33.21455</v>
+      </c>
+      <c r="M38" t="n">
+        <v>90</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>17.582275</v>
+      </c>
+      <c r="P38" t="n">
+        <v>17.9152125</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>2</v>
+      </c>
+      <c r="S38" t="n">
+        <v>90760</v>
+      </c>
+      <c r="T38" t="n">
+        <v>3.697421966131398e-05</v>
+      </c>
+      <c r="U38" t="b">
+        <v>1</v>
+      </c>
+      <c r="V38" t="n">
+        <v>29</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0</v>
+      </c>
+      <c r="X38" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>400</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB38" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC38" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD38" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE38" t="inlineStr"/>
+      <c r="AF38" t="n">
+        <v>0.01031832868477658</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>4932</v>
+      </c>
+      <c r="C39" t="n">
+        <v>37</v>
+      </c>
+      <c r="D39" t="n">
+        <v>-0.58859375</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.0009375</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2.222145808576915</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.1482470085477335</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.001982496444074563</v>
+      </c>
+      <c r="I39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>2.050008547542936</v>
+      </c>
+      <c r="L39" t="n">
+        <v>33.6229</v>
+      </c>
+      <c r="M39" t="n">
+        <v>90</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>18.036325</v>
+      </c>
+      <c r="P39" t="n">
+        <v>17.92435</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>2</v>
+      </c>
+      <c r="S39" t="n">
+        <v>91547</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0.01254329515847652</v>
+      </c>
+      <c r="U39" t="b">
+        <v>1</v>
+      </c>
+      <c r="V39" t="n">
+        <v>31</v>
+      </c>
+      <c r="W39" t="n">
+        <v>147</v>
+      </c>
+      <c r="X39" t="n">
+        <v>120</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>122</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>1.299999999999999</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB39" t="inlineStr">
+        <is>
+          <t>atq</t>
+        </is>
+      </c>
+      <c r="AC39" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD39" t="inlineStr">
+        <is>
+          <t>vincent</t>
+        </is>
+      </c>
+      <c r="AE39" t="n">
+        <v>0.5409029329571727</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>0.01060528634485899</v>
+      </c>
+      <c r="AG39" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>